<commit_message>
- Export updated data of Member (current residency and marital status) - Fix Household Proxy Head ODK Form by adding missing options
</commit_message>
<xml_diff>
--- a/src/main/resources/samples/extension-forms/xls/household_proxy_head_ext.xlsx
+++ b/src/main/resources/samples/extension-forms/xls/household_proxy_head_ext.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="27795" windowHeight="12195" activeTab="2"/>
+    <workbookView windowWidth="27795" windowHeight="12195"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="166">
   <si>
     <t>type</t>
   </si>
@@ -141,6 +141,9 @@
     <t>Nome do Agregado</t>
   </si>
   <si>
+    <t>select_one proxy_head_types</t>
+  </si>
+  <si>
     <t>proxy_head_type</t>
   </si>
   <si>
@@ -168,6 +171,9 @@
     <t>Nome do Chefe Substituto</t>
   </si>
   <si>
+    <t>select_one proxy_head_roles</t>
+  </si>
+  <si>
     <t>proxy_head_role</t>
   </si>
   <si>
@@ -343,6 +349,147 @@
   </si>
   <si>
     <t>Aborto induzido</t>
+  </si>
+  <si>
+    <t>proxy_head_types</t>
+  </si>
+  <si>
+    <t>RESIDENT</t>
+  </si>
+  <si>
+    <t>Resident Proxy Head</t>
+  </si>
+  <si>
+    <t>Chefe Substituto Residente</t>
+  </si>
+  <si>
+    <t>NON_RESIDENT</t>
+  </si>
+  <si>
+    <t>Non-resident Proxy Head (registered in DSS, different household)</t>
+  </si>
+  <si>
+    <t>Chefe Substituto Não Residente (reside noutro agregado)</t>
+  </si>
+  <si>
+    <t>NON_DSS_MEMBER</t>
+  </si>
+  <si>
+    <t>Non-DSS Member Proxy Head (external to the system)</t>
+  </si>
+  <si>
+    <t>Não é Membro do DSS</t>
+  </si>
+  <si>
+    <t>proxy_head_roles</t>
+  </si>
+  <si>
+    <t>ADM</t>
+  </si>
+  <si>
+    <t>Administrator</t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t>WRD</t>
+  </si>
+  <si>
+    <t>Warden</t>
+  </si>
+  <si>
+    <t>Guarda</t>
+  </si>
+  <si>
+    <t>SOC</t>
+  </si>
+  <si>
+    <t>Social Worker</t>
+  </si>
+  <si>
+    <t>Assistente Social</t>
+  </si>
+  <si>
+    <t>CTK</t>
+  </si>
+  <si>
+    <t>Caretaker</t>
+  </si>
+  <si>
+    <t>Cuidador</t>
+  </si>
+  <si>
+    <t>LGU</t>
+  </si>
+  <si>
+    <t>Legal Guardian</t>
+  </si>
+  <si>
+    <t>Tutor Legal</t>
+  </si>
+  <si>
+    <t>FAM</t>
+  </si>
+  <si>
+    <t>Family Representative</t>
+  </si>
+  <si>
+    <t>Representante da Família</t>
+  </si>
+  <si>
+    <t>COM</t>
+  </si>
+  <si>
+    <t>Community Representative</t>
+  </si>
+  <si>
+    <t>Representante da Comunidade</t>
+  </si>
+  <si>
+    <t>REL</t>
+  </si>
+  <si>
+    <t>Religious Leader</t>
+  </si>
+  <si>
+    <t>Líder Religioso</t>
+  </si>
+  <si>
+    <t>MIL</t>
+  </si>
+  <si>
+    <t>Military Commander</t>
+  </si>
+  <si>
+    <t>Comandante Militar</t>
+  </si>
+  <si>
+    <t>PRI</t>
+  </si>
+  <si>
+    <t>Principal</t>
+  </si>
+  <si>
+    <t>Diretor da Escola</t>
+  </si>
+  <si>
+    <t>DIR</t>
+  </si>
+  <si>
+    <t>Director</t>
+  </si>
+  <si>
+    <t>Diretor</t>
+  </si>
+  <si>
+    <t>OTH</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Outro</t>
   </si>
   <si>
     <t>form_title</t>
@@ -377,8 +524,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -425,11 +572,64 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -442,30 +642,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -481,21 +658,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -503,7 +665,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -511,14 +673,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -532,15 +686,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -554,22 +709,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -579,6 +726,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -596,7 +749,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -608,7 +767,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -620,7 +797,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -632,139 +905,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -776,7 +917,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -787,6 +940,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -829,17 +997,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -851,15 +1013,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -882,8 +1035,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -891,159 +1044,159 @@
   <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1090,6 +1243,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1114,13 +1284,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -1129,31 +1299,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1516,12 +1686,12 @@
   <sheetPr/>
   <dimension ref="A1:V57"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -1545,221 +1715,221 @@
     <col min="18" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" s="25" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
-      <c r="A1" s="29" t="s">
+    <row r="1" s="34" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="K1" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="29" t="s">
+      <c r="L1" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="29" t="s">
+      <c r="M1" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="29" t="s">
+      <c r="O1" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="29" t="s">
+      <c r="P1" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="29" t="s">
+      <c r="Q1" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="29" t="s">
+      <c r="R1" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="29" t="s">
+      <c r="S1" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="29" t="s">
+      <c r="T1" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="29" t="s">
+      <c r="U1" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="29" t="s">
+      <c r="V1" s="38" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" s="26" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
-      <c r="A2" s="31" t="s">
+    <row r="2" s="35" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
+      <c r="A2" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="37" t="s">
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34"/>
-      <c r="V2" s="34"/>
-    </row>
-    <row r="3" s="26" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
-      <c r="A3" s="31" t="s">
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="43"/>
+      <c r="V2" s="43"/>
+    </row>
+    <row r="3" s="35" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
+      <c r="A3" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="37" t="s">
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="34"/>
-      <c r="P3" s="34"/>
-      <c r="Q3" s="34"/>
-      <c r="R3" s="34"/>
-      <c r="S3" s="34"/>
-      <c r="T3" s="34"/>
-      <c r="U3" s="34"/>
-      <c r="V3" s="34"/>
-    </row>
-    <row r="4" s="26" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
-      <c r="A4" s="31" t="s">
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="43"/>
+      <c r="S3" s="43"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="43"/>
+      <c r="V3" s="43"/>
+    </row>
+    <row r="4" s="35" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
+      <c r="A4" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="37" t="s">
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="34"/>
-      <c r="P4" s="34"/>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="34"/>
-      <c r="S4" s="34"/>
-      <c r="T4" s="34"/>
-      <c r="U4" s="34"/>
-      <c r="V4" s="34"/>
-    </row>
-    <row r="5" s="27" customFormat="1" spans="1:14">
-      <c r="A5" s="27" t="s">
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="43"/>
+      <c r="T4" s="43"/>
+      <c r="U4" s="43"/>
+      <c r="V4" s="43"/>
+    </row>
+    <row r="5" s="36" customFormat="1" spans="1:14">
+      <c r="A5" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="38" t="s">
+      <c r="J5" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="N5" s="38" t="s">
+      <c r="N5" s="47" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" s="27" customFormat="1" spans="1:14">
-      <c r="A6" s="27" t="s">
+    <row r="6" s="36" customFormat="1" spans="1:14">
+      <c r="A6" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="42" t="s">
         <v>32</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="38" t="s">
+      <c r="J6" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="N6" s="38" t="s">
+      <c r="N6" s="47" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" s="27" customFormat="1" spans="1:14">
-      <c r="A7" s="27" t="s">
+    <row r="7" s="36" customFormat="1" spans="1:14">
+      <c r="A7" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="36" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -1768,18 +1938,18 @@
       <c r="D7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="J7" s="38" t="s">
+      <c r="J7" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="N7" s="38" t="s">
+      <c r="N7" s="47" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" s="27" customFormat="1" spans="1:14">
-      <c r="A8" s="27" t="s">
+    <row r="8" s="36" customFormat="1" spans="1:14">
+      <c r="A8" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="36" t="s">
         <v>37</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -1788,305 +1958,305 @@
       <c r="D8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="38" t="s">
+      <c r="J8" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="N8" s="38" t="s">
+      <c r="N8" s="47" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" s="27" customFormat="1" customHeight="1" spans="1:14">
-      <c r="A9" s="27" t="s">
+    <row r="9" s="36" customFormat="1" customHeight="1" spans="1:14">
+      <c r="A9" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="N9" s="47" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" s="36" customFormat="1" customHeight="1" spans="1:14">
+      <c r="A10" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J9" s="38" t="s">
+      <c r="B10" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="N9" s="38" t="s">
+      <c r="N10" s="47" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" s="27" customFormat="1" customHeight="1" spans="1:14">
-      <c r="A10" s="27" t="s">
+    <row r="11" s="36" customFormat="1" spans="1:14">
+      <c r="A11" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="J10" s="38" t="s">
+      <c r="B11" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="N10" s="38" t="s">
+      <c r="N11" s="47" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" s="27" customFormat="1" spans="1:14">
-      <c r="A11" s="27" t="s">
+    <row r="12" s="36" customFormat="1" spans="1:14">
+      <c r="A12" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="N12" s="47" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" s="37" customFormat="1" spans="1:14">
+      <c r="A13" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J11" s="38" t="s">
-        <v>24</v>
-      </c>
-      <c r="N11" s="38" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" s="27" customFormat="1" spans="1:14">
-      <c r="A12" s="27" t="s">
+      <c r="B13" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="J13" s="48"/>
+      <c r="N13" s="48"/>
+    </row>
+    <row r="14" s="37" customFormat="1" customHeight="1" spans="1:14">
+      <c r="A14" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="J12" s="38" t="s">
-        <v>24</v>
-      </c>
-      <c r="N12" s="38" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" s="28" customFormat="1" spans="1:14">
-      <c r="A13" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="J13" s="39"/>
-      <c r="N13" s="39"/>
-    </row>
-    <row r="14" s="28" customFormat="1" customHeight="1" spans="1:14">
-      <c r="A14" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="J14" s="39"/>
-      <c r="N14" s="39"/>
-    </row>
-    <row r="15" s="27" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J15" s="38"/>
-      <c r="N15" s="38"/>
-    </row>
-    <row r="16" s="27" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J16" s="38"/>
-      <c r="N16" s="38"/>
-    </row>
-    <row r="17" s="27" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J17" s="38"/>
-      <c r="N17" s="38"/>
-    </row>
-    <row r="18" s="27" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J18" s="38"/>
-      <c r="N18" s="38"/>
-    </row>
-    <row r="19" s="27" customFormat="1" spans="10:14">
-      <c r="J19" s="38"/>
-      <c r="N19" s="38"/>
-    </row>
-    <row r="20" s="27" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J20" s="38"/>
-      <c r="N20" s="38"/>
-    </row>
-    <row r="21" s="27" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J21" s="38"/>
-      <c r="N21" s="38"/>
-    </row>
-    <row r="22" s="27" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J22" s="38"/>
-      <c r="N22" s="38"/>
-    </row>
-    <row r="23" s="27" customFormat="1" spans="10:14">
-      <c r="J23" s="38"/>
-      <c r="N23" s="38"/>
-    </row>
-    <row r="24" s="27" customFormat="1" spans="10:14">
-      <c r="J24" s="38"/>
-      <c r="N24" s="38"/>
-    </row>
-    <row r="25" s="27" customFormat="1" spans="10:14">
-      <c r="J25" s="38"/>
-      <c r="N25" s="38"/>
-    </row>
-    <row r="26" s="27" customFormat="1" ht="15.75" customHeight="1" spans="10:14">
-      <c r="J26" s="38"/>
-      <c r="N26" s="38"/>
-    </row>
-    <row r="27" s="27" customFormat="1" ht="13.5" customHeight="1" spans="10:14">
-      <c r="J27" s="38"/>
-      <c r="N27" s="38"/>
-    </row>
-    <row r="28" s="27" customFormat="1" spans="10:14">
-      <c r="J28" s="38"/>
-      <c r="N28" s="38"/>
-    </row>
-    <row r="29" s="27" customFormat="1" spans="10:14">
-      <c r="J29" s="38"/>
-      <c r="N29" s="38"/>
-    </row>
-    <row r="30" s="27" customFormat="1" spans="10:14">
-      <c r="J30" s="38"/>
-      <c r="N30" s="38"/>
-    </row>
-    <row r="31" s="27" customFormat="1" ht="13.5" customHeight="1" spans="10:14">
-      <c r="J31" s="38"/>
-      <c r="N31" s="38"/>
-    </row>
-    <row r="32" s="27" customFormat="1" spans="10:14">
-      <c r="J32" s="38"/>
-      <c r="N32" s="38"/>
-    </row>
-    <row r="33" s="27" customFormat="1" spans="10:14">
-      <c r="J33" s="38"/>
-      <c r="N33" s="38"/>
-    </row>
-    <row r="34" s="27" customFormat="1" spans="10:14">
-      <c r="J34" s="38"/>
-      <c r="N34" s="38"/>
-    </row>
-    <row r="35" s="27" customFormat="1" spans="10:14">
-      <c r="J35" s="38"/>
-      <c r="N35" s="38"/>
-    </row>
-    <row r="36" s="27" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J36" s="38"/>
-      <c r="N36" s="38"/>
-    </row>
-    <row r="37" s="27" customFormat="1" ht="12" customHeight="1" spans="10:14">
-      <c r="J37" s="38"/>
-      <c r="N37" s="38"/>
-    </row>
-    <row r="38" s="27" customFormat="1" spans="10:14">
-      <c r="J38" s="38"/>
-      <c r="N38" s="38"/>
-    </row>
-    <row r="39" s="27" customFormat="1" spans="10:14">
-      <c r="J39" s="38"/>
-      <c r="N39" s="38"/>
-    </row>
-    <row r="40" s="27" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J40" s="38"/>
-      <c r="N40" s="38"/>
-    </row>
-    <row r="41" s="27" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J41" s="38"/>
-      <c r="N41" s="38"/>
-    </row>
-    <row r="42" s="27" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J42" s="38"/>
-      <c r="N42" s="38"/>
-    </row>
-    <row r="43" s="27" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J43" s="38"/>
-      <c r="N43" s="38"/>
-    </row>
-    <row r="44" s="27" customFormat="1" spans="10:14">
-      <c r="J44" s="38"/>
-      <c r="N44" s="38"/>
-    </row>
-    <row r="45" s="27" customFormat="1" spans="10:14">
-      <c r="J45" s="38"/>
-      <c r="N45" s="38"/>
-    </row>
-    <row r="46" s="27" customFormat="1" spans="10:14">
-      <c r="J46" s="38"/>
-      <c r="N46" s="38"/>
-    </row>
-    <row r="47" s="27" customFormat="1" spans="10:14">
-      <c r="J47" s="38"/>
-      <c r="N47" s="38"/>
-    </row>
-    <row r="48" s="27" customFormat="1" spans="10:14">
-      <c r="J48" s="38"/>
-      <c r="N48" s="38"/>
-    </row>
-    <row r="49" s="27" customFormat="1" spans="10:14">
-      <c r="J49" s="38"/>
-      <c r="N49" s="38"/>
-    </row>
-    <row r="50" s="27" customFormat="1" spans="10:14">
-      <c r="J50" s="38"/>
-      <c r="N50" s="38"/>
-    </row>
-    <row r="51" s="27" customFormat="1" spans="10:14">
-      <c r="J51" s="38"/>
-      <c r="N51" s="38"/>
-    </row>
-    <row r="52" s="27" customFormat="1" spans="10:14">
-      <c r="J52" s="38"/>
-      <c r="N52" s="38"/>
-    </row>
-    <row r="53" s="27" customFormat="1" spans="10:14">
-      <c r="J53" s="38"/>
-      <c r="N53" s="38"/>
-    </row>
-    <row r="54" s="27" customFormat="1" spans="10:14">
-      <c r="J54" s="38"/>
-      <c r="N54" s="38"/>
-    </row>
-    <row r="55" s="27" customFormat="1" spans="10:14">
-      <c r="J55" s="38"/>
-      <c r="N55" s="38"/>
-    </row>
-    <row r="56" s="27" customFormat="1" spans="10:14">
-      <c r="J56" s="38"/>
-      <c r="N56" s="38"/>
+      <c r="B14" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="J14" s="48"/>
+      <c r="N14" s="48"/>
+    </row>
+    <row r="15" s="36" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J15" s="47"/>
+      <c r="N15" s="47"/>
+    </row>
+    <row r="16" s="36" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J16" s="47"/>
+      <c r="N16" s="47"/>
+    </row>
+    <row r="17" s="36" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J17" s="47"/>
+      <c r="N17" s="47"/>
+    </row>
+    <row r="18" s="36" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J18" s="47"/>
+      <c r="N18" s="47"/>
+    </row>
+    <row r="19" s="36" customFormat="1" spans="10:14">
+      <c r="J19" s="47"/>
+      <c r="N19" s="47"/>
+    </row>
+    <row r="20" s="36" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J20" s="47"/>
+      <c r="N20" s="47"/>
+    </row>
+    <row r="21" s="36" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J21" s="47"/>
+      <c r="N21" s="47"/>
+    </row>
+    <row r="22" s="36" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J22" s="47"/>
+      <c r="N22" s="47"/>
+    </row>
+    <row r="23" s="36" customFormat="1" spans="10:14">
+      <c r="J23" s="47"/>
+      <c r="N23" s="47"/>
+    </row>
+    <row r="24" s="36" customFormat="1" spans="10:14">
+      <c r="J24" s="47"/>
+      <c r="N24" s="47"/>
+    </row>
+    <row r="25" s="36" customFormat="1" spans="10:14">
+      <c r="J25" s="47"/>
+      <c r="N25" s="47"/>
+    </row>
+    <row r="26" s="36" customFormat="1" ht="15.75" customHeight="1" spans="10:14">
+      <c r="J26" s="47"/>
+      <c r="N26" s="47"/>
+    </row>
+    <row r="27" s="36" customFormat="1" ht="13.5" customHeight="1" spans="10:14">
+      <c r="J27" s="47"/>
+      <c r="N27" s="47"/>
+    </row>
+    <row r="28" s="36" customFormat="1" spans="10:14">
+      <c r="J28" s="47"/>
+      <c r="N28" s="47"/>
+    </row>
+    <row r="29" s="36" customFormat="1" spans="10:14">
+      <c r="J29" s="47"/>
+      <c r="N29" s="47"/>
+    </row>
+    <row r="30" s="36" customFormat="1" spans="10:14">
+      <c r="J30" s="47"/>
+      <c r="N30" s="47"/>
+    </row>
+    <row r="31" s="36" customFormat="1" ht="13.5" customHeight="1" spans="10:14">
+      <c r="J31" s="47"/>
+      <c r="N31" s="47"/>
+    </row>
+    <row r="32" s="36" customFormat="1" spans="10:14">
+      <c r="J32" s="47"/>
+      <c r="N32" s="47"/>
+    </row>
+    <row r="33" s="36" customFormat="1" spans="10:14">
+      <c r="J33" s="47"/>
+      <c r="N33" s="47"/>
+    </row>
+    <row r="34" s="36" customFormat="1" spans="10:14">
+      <c r="J34" s="47"/>
+      <c r="N34" s="47"/>
+    </row>
+    <row r="35" s="36" customFormat="1" spans="10:14">
+      <c r="J35" s="47"/>
+      <c r="N35" s="47"/>
+    </row>
+    <row r="36" s="36" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J36" s="47"/>
+      <c r="N36" s="47"/>
+    </row>
+    <row r="37" s="36" customFormat="1" ht="12" customHeight="1" spans="10:14">
+      <c r="J37" s="47"/>
+      <c r="N37" s="47"/>
+    </row>
+    <row r="38" s="36" customFormat="1" spans="10:14">
+      <c r="J38" s="47"/>
+      <c r="N38" s="47"/>
+    </row>
+    <row r="39" s="36" customFormat="1" spans="10:14">
+      <c r="J39" s="47"/>
+      <c r="N39" s="47"/>
+    </row>
+    <row r="40" s="36" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J40" s="47"/>
+      <c r="N40" s="47"/>
+    </row>
+    <row r="41" s="36" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J41" s="47"/>
+      <c r="N41" s="47"/>
+    </row>
+    <row r="42" s="36" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J42" s="47"/>
+      <c r="N42" s="47"/>
+    </row>
+    <row r="43" s="36" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J43" s="47"/>
+      <c r="N43" s="47"/>
+    </row>
+    <row r="44" s="36" customFormat="1" spans="10:14">
+      <c r="J44" s="47"/>
+      <c r="N44" s="47"/>
+    </row>
+    <row r="45" s="36" customFormat="1" spans="10:14">
+      <c r="J45" s="47"/>
+      <c r="N45" s="47"/>
+    </row>
+    <row r="46" s="36" customFormat="1" spans="10:14">
+      <c r="J46" s="47"/>
+      <c r="N46" s="47"/>
+    </row>
+    <row r="47" s="36" customFormat="1" spans="10:14">
+      <c r="J47" s="47"/>
+      <c r="N47" s="47"/>
+    </row>
+    <row r="48" s="36" customFormat="1" spans="10:14">
+      <c r="J48" s="47"/>
+      <c r="N48" s="47"/>
+    </row>
+    <row r="49" s="36" customFormat="1" spans="10:14">
+      <c r="J49" s="47"/>
+      <c r="N49" s="47"/>
+    </row>
+    <row r="50" s="36" customFormat="1" spans="10:14">
+      <c r="J50" s="47"/>
+      <c r="N50" s="47"/>
+    </row>
+    <row r="51" s="36" customFormat="1" spans="10:14">
+      <c r="J51" s="47"/>
+      <c r="N51" s="47"/>
+    </row>
+    <row r="52" s="36" customFormat="1" spans="10:14">
+      <c r="J52" s="47"/>
+      <c r="N52" s="47"/>
+    </row>
+    <row r="53" s="36" customFormat="1" spans="10:14">
+      <c r="J53" s="47"/>
+      <c r="N53" s="47"/>
+    </row>
+    <row r="54" s="36" customFormat="1" spans="10:14">
+      <c r="J54" s="47"/>
+      <c r="N54" s="47"/>
+    </row>
+    <row r="55" s="36" customFormat="1" spans="10:14">
+      <c r="J55" s="47"/>
+      <c r="N55" s="47"/>
+    </row>
+    <row r="56" s="36" customFormat="1" spans="10:14">
+      <c r="J56" s="47"/>
+      <c r="N56" s="47"/>
     </row>
     <row r="57" spans="1:11">
-      <c r="A57" s="27"/>
-      <c r="B57" s="27"/>
-      <c r="C57" s="27"/>
-      <c r="D57" s="27"/>
-      <c r="E57" s="27"/>
-      <c r="F57" s="27"/>
-      <c r="G57" s="27"/>
-      <c r="H57" s="27"/>
-      <c r="I57" s="27"/>
-      <c r="J57" s="38"/>
-      <c r="K57" s="27"/>
+      <c r="A57" s="36"/>
+      <c r="B57" s="36"/>
+      <c r="C57" s="36"/>
+      <c r="D57" s="36"/>
+      <c r="E57" s="36"/>
+      <c r="F57" s="36"/>
+      <c r="G57" s="36"/>
+      <c r="H57" s="36"/>
+      <c r="I57" s="36"/>
+      <c r="J57" s="47"/>
+      <c r="K57" s="36"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -2107,30 +2277,30 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.6333333333333" defaultRowHeight="14.25" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="16.5416666666667" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.5416666666667" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.75" style="5" customWidth="1"/>
-    <col min="4" max="4" width="24.125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="52.75" style="5" customWidth="1"/>
+    <col min="4" max="4" width="46.25" style="4" customWidth="1"/>
     <col min="5" max="16384" width="13.6333333333333" style="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:5">
       <c r="A1" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>17</v>
@@ -2138,288 +2308,423 @@
     </row>
     <row r="2" ht="12.75" customHeight="1" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B2" s="8">
         <v>1</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B3" s="8">
         <v>0</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="13" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="13" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="13" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="11" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="11" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="11" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="11" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="6"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="6"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="6"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="6"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="6"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="6"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="6"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="6"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="6"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="6"/>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="6"/>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="6"/>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="6"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="17"/>
@@ -2569,17 +2874,17 @@
     <row r="61" ht="15" spans="1:3">
       <c r="A61" s="17"/>
       <c r="B61" s="17"/>
-      <c r="C61" s="18"/>
+      <c r="C61" s="27"/>
     </row>
     <row r="62" ht="15" spans="1:3">
       <c r="A62" s="17"/>
       <c r="B62" s="17"/>
-      <c r="C62" s="18"/>
+      <c r="C62" s="27"/>
     </row>
     <row r="63" ht="15" spans="1:3">
       <c r="A63" s="17"/>
       <c r="B63" s="17"/>
-      <c r="C63" s="18"/>
+      <c r="C63" s="27"/>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="17"/>
@@ -2805,44 +3110,44 @@
       <c r="A108" s="17"/>
       <c r="B108" s="17"/>
       <c r="C108" s="6"/>
-      <c r="D108" s="19"/>
+      <c r="D108" s="28"/>
       <c r="E108"/>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="17"/>
       <c r="B109" s="17"/>
       <c r="C109" s="6"/>
-      <c r="D109" s="19"/>
+      <c r="D109" s="28"/>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="17"/>
       <c r="B110" s="17"/>
       <c r="C110" s="6"/>
-      <c r="D110" s="19"/>
+      <c r="D110" s="28"/>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="17"/>
       <c r="B111" s="17"/>
       <c r="C111" s="6"/>
-      <c r="D111" s="19"/>
+      <c r="D111" s="28"/>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="17"/>
       <c r="B112" s="17"/>
       <c r="C112" s="6"/>
-      <c r="D112" s="19"/>
+      <c r="D112" s="28"/>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="17"/>
       <c r="B113" s="17"/>
       <c r="C113" s="6"/>
-      <c r="D113" s="19"/>
+      <c r="D113" s="28"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="17"/>
       <c r="B114" s="17"/>
       <c r="C114" s="6"/>
-      <c r="D114" s="19"/>
+      <c r="D114" s="28"/>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" s="17"/>
@@ -2910,247 +3215,247 @@
       <c r="C127" s="6"/>
     </row>
     <row r="128" spans="3:3">
-      <c r="C128" s="20"/>
+      <c r="C128" s="29"/>
     </row>
     <row r="129" spans="3:3">
-      <c r="C129" s="20"/>
+      <c r="C129" s="29"/>
     </row>
     <row r="130" spans="3:3">
-      <c r="C130" s="20"/>
+      <c r="C130" s="29"/>
     </row>
     <row r="131" spans="3:3">
-      <c r="C131" s="20"/>
+      <c r="C131" s="29"/>
     </row>
     <row r="132" spans="3:3">
-      <c r="C132" s="20"/>
+      <c r="C132" s="29"/>
     </row>
     <row r="133" spans="3:3">
-      <c r="C133" s="20"/>
+      <c r="C133" s="29"/>
     </row>
     <row r="134" spans="3:3">
       <c r="C134" s="6"/>
     </row>
     <row r="135" spans="3:3">
-      <c r="C135" s="20"/>
+      <c r="C135" s="29"/>
     </row>
     <row r="136" spans="3:3">
-      <c r="C136" s="20"/>
+      <c r="C136" s="29"/>
     </row>
     <row r="137" spans="3:3">
-      <c r="C137" s="20"/>
+      <c r="C137" s="29"/>
     </row>
     <row r="138" spans="3:3">
-      <c r="C138" s="20"/>
+      <c r="C138" s="29"/>
     </row>
     <row r="139" spans="3:3">
-      <c r="C139" s="20"/>
+      <c r="C139" s="29"/>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="3"/>
-      <c r="C140" s="21"/>
+      <c r="C140" s="30"/>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="3"/>
-      <c r="C141" s="21"/>
+      <c r="C141" s="30"/>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" s="3"/>
-      <c r="C142" s="21"/>
+      <c r="C142" s="30"/>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="3"/>
-      <c r="C143" s="21"/>
+      <c r="C143" s="30"/>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="3"/>
-      <c r="C144" s="21"/>
+      <c r="C144" s="30"/>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" s="3"/>
-      <c r="C145" s="21"/>
+      <c r="C145" s="30"/>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="3"/>
-      <c r="C146" s="21"/>
+      <c r="C146" s="30"/>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="3"/>
-      <c r="C147" s="21"/>
+      <c r="C147" s="30"/>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" s="3"/>
-      <c r="C148" s="21"/>
+      <c r="C148" s="30"/>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="3"/>
-      <c r="C149" s="21"/>
+      <c r="C149" s="30"/>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" s="3"/>
-      <c r="C150" s="21"/>
+      <c r="C150" s="30"/>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" s="3"/>
-      <c r="C151" s="21"/>
+      <c r="C151" s="30"/>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" s="3"/>
-      <c r="C152" s="21"/>
+      <c r="C152" s="30"/>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" s="3"/>
-      <c r="C153" s="21"/>
+      <c r="C153" s="30"/>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" s="3"/>
-      <c r="C154" s="21"/>
+      <c r="C154" s="30"/>
     </row>
     <row r="155" spans="3:4">
-      <c r="C155" s="20"/>
-      <c r="D155" s="20"/>
+      <c r="C155" s="29"/>
+      <c r="D155" s="29"/>
     </row>
     <row r="156" spans="3:4">
-      <c r="C156" s="20"/>
-      <c r="D156" s="20"/>
+      <c r="C156" s="29"/>
+      <c r="D156" s="29"/>
     </row>
     <row r="157" spans="3:4">
-      <c r="C157" s="20"/>
-      <c r="D157" s="20"/>
+      <c r="C157" s="29"/>
+      <c r="D157" s="29"/>
     </row>
     <row r="158" spans="3:4">
-      <c r="C158" s="20"/>
-      <c r="D158" s="20"/>
+      <c r="C158" s="29"/>
+      <c r="D158" s="29"/>
     </row>
     <row r="159" spans="3:4">
-      <c r="C159" s="20"/>
-      <c r="D159" s="20"/>
+      <c r="C159" s="29"/>
+      <c r="D159" s="29"/>
     </row>
     <row r="160" spans="3:4">
-      <c r="C160" s="20"/>
-      <c r="D160" s="20"/>
+      <c r="C160" s="29"/>
+      <c r="D160" s="29"/>
     </row>
     <row r="161" spans="3:4">
-      <c r="C161" s="20"/>
-      <c r="D161" s="20"/>
+      <c r="C161" s="29"/>
+      <c r="D161" s="29"/>
     </row>
     <row r="162" spans="3:4">
-      <c r="C162" s="20"/>
-      <c r="D162" s="20"/>
+      <c r="C162" s="29"/>
+      <c r="D162" s="29"/>
     </row>
     <row r="163" spans="3:4">
       <c r="C163" s="6"/>
       <c r="D163" s="6"/>
     </row>
     <row r="164" spans="3:3">
-      <c r="C164" s="20"/>
+      <c r="C164" s="29"/>
     </row>
     <row r="165" spans="3:3">
-      <c r="C165" s="20"/>
+      <c r="C165" s="29"/>
     </row>
     <row r="166" spans="3:3">
-      <c r="C166" s="20"/>
+      <c r="C166" s="29"/>
     </row>
     <row r="167" spans="3:3">
-      <c r="C167" s="20"/>
+      <c r="C167" s="29"/>
     </row>
     <row r="168" spans="3:3">
-      <c r="C168" s="20"/>
+      <c r="C168" s="29"/>
     </row>
     <row r="169" spans="3:3">
-      <c r="C169" s="20"/>
+      <c r="C169" s="29"/>
     </row>
     <row r="170" spans="3:3">
-      <c r="C170" s="20"/>
+      <c r="C170" s="29"/>
     </row>
     <row r="171" spans="3:3">
-      <c r="C171" s="20"/>
+      <c r="C171" s="29"/>
     </row>
     <row r="172" spans="3:3">
-      <c r="C172" s="20"/>
+      <c r="C172" s="29"/>
     </row>
     <row r="173" spans="3:3">
-      <c r="C173" s="20"/>
+      <c r="C173" s="29"/>
     </row>
     <row r="174" spans="3:3">
-      <c r="C174" s="20"/>
+      <c r="C174" s="29"/>
     </row>
     <row r="175" spans="3:3">
-      <c r="C175" s="20"/>
+      <c r="C175" s="29"/>
     </row>
     <row r="176" spans="3:3">
-      <c r="C176" s="20"/>
+      <c r="C176" s="29"/>
     </row>
     <row r="177" spans="3:3">
-      <c r="C177" s="20"/>
+      <c r="C177" s="29"/>
     </row>
     <row r="178" spans="3:3">
-      <c r="C178" s="20"/>
+      <c r="C178" s="29"/>
     </row>
     <row r="195" spans="3:3">
-      <c r="C195" s="20"/>
+      <c r="C195" s="29"/>
     </row>
     <row r="196" spans="3:3">
-      <c r="C196" s="20"/>
+      <c r="C196" s="29"/>
     </row>
     <row r="197" spans="3:3">
-      <c r="C197" s="20"/>
+      <c r="C197" s="29"/>
     </row>
     <row r="198" spans="3:3">
-      <c r="C198" s="20"/>
+      <c r="C198" s="29"/>
     </row>
     <row r="199" spans="3:3">
-      <c r="C199" s="20"/>
+      <c r="C199" s="29"/>
     </row>
     <row r="200" spans="3:3">
-      <c r="C200" s="20"/>
+      <c r="C200" s="29"/>
     </row>
     <row r="201" spans="3:3">
-      <c r="C201" s="20"/>
+      <c r="C201" s="29"/>
     </row>
     <row r="202" spans="3:3">
-      <c r="C202" s="20"/>
+      <c r="C202" s="29"/>
     </row>
     <row r="203" spans="3:3">
-      <c r="C203" s="20"/>
+      <c r="C203" s="29"/>
     </row>
     <row r="204" spans="3:3">
-      <c r="C204" s="20"/>
+      <c r="C204" s="29"/>
     </row>
     <row r="205" spans="3:3">
-      <c r="C205" s="20"/>
+      <c r="C205" s="29"/>
     </row>
     <row r="206" spans="3:3">
-      <c r="C206" s="20"/>
+      <c r="C206" s="29"/>
     </row>
     <row r="207" spans="3:3">
-      <c r="C207" s="20"/>
+      <c r="C207" s="29"/>
     </row>
     <row r="208" spans="3:3">
-      <c r="C208" s="20"/>
+      <c r="C208" s="29"/>
     </row>
     <row r="209" spans="3:3">
-      <c r="C209" s="20"/>
+      <c r="C209" s="29"/>
     </row>
     <row r="210" spans="3:3">
-      <c r="C210" s="20"/>
+      <c r="C210" s="29"/>
     </row>
     <row r="211" spans="3:3">
-      <c r="C211" s="20"/>
+      <c r="C211" s="29"/>
     </row>
     <row r="212" spans="3:3">
-      <c r="C212" s="20"/>
+      <c r="C212" s="29"/>
     </row>
     <row r="213" spans="3:3">
-      <c r="C213" s="20"/>
+      <c r="C213" s="29"/>
     </row>
     <row r="225" spans="3:3">
-      <c r="C225" s="22"/>
+      <c r="C225" s="31"/>
     </row>
     <row r="226" spans="3:3">
-      <c r="C226" s="22"/>
+      <c r="C226" s="31"/>
     </row>
     <row r="227" spans="3:3">
-      <c r="C227" s="23"/>
+      <c r="C227" s="32"/>
     </row>
     <row r="236" spans="3:3">
       <c r="C236" s="4"/>
@@ -3252,487 +3557,487 @@
       <c r="C268" s="4"/>
     </row>
     <row r="269" spans="3:3">
-      <c r="C269" s="19"/>
+      <c r="C269" s="28"/>
     </row>
     <row r="270" spans="3:3">
-      <c r="C270" s="19"/>
+      <c r="C270" s="28"/>
     </row>
     <row r="271" spans="3:3">
-      <c r="C271" s="19"/>
+      <c r="C271" s="28"/>
     </row>
     <row r="272" spans="3:3">
-      <c r="C272" s="19"/>
+      <c r="C272" s="28"/>
     </row>
     <row r="273" spans="3:3">
-      <c r="C273" s="19"/>
+      <c r="C273" s="28"/>
     </row>
     <row r="274" spans="3:3">
-      <c r="C274" s="19"/>
+      <c r="C274" s="28"/>
     </row>
     <row r="275" spans="3:3">
-      <c r="C275" s="19"/>
+      <c r="C275" s="28"/>
     </row>
     <row r="276" spans="3:3">
-      <c r="C276" s="19"/>
+      <c r="C276" s="28"/>
     </row>
     <row r="277" spans="3:3">
-      <c r="C277" s="19"/>
+      <c r="C277" s="28"/>
     </row>
     <row r="278" spans="3:3">
-      <c r="C278" s="19"/>
+      <c r="C278" s="28"/>
     </row>
     <row r="279" spans="3:3">
-      <c r="C279" s="19"/>
+      <c r="C279" s="28"/>
     </row>
     <row r="280" spans="3:3">
-      <c r="C280" s="19"/>
+      <c r="C280" s="28"/>
     </row>
     <row r="281" spans="3:3">
-      <c r="C281" s="19"/>
+      <c r="C281" s="28"/>
     </row>
     <row r="282" spans="3:3">
-      <c r="C282" s="19"/>
+      <c r="C282" s="28"/>
     </row>
     <row r="283" spans="3:3">
-      <c r="C283" s="19"/>
+      <c r="C283" s="28"/>
     </row>
     <row r="284" spans="3:3">
-      <c r="C284" s="19"/>
+      <c r="C284" s="28"/>
     </row>
     <row r="285" spans="3:3">
-      <c r="C285" s="19"/>
+      <c r="C285" s="28"/>
     </row>
     <row r="286" spans="3:3">
-      <c r="C286" s="19"/>
+      <c r="C286" s="28"/>
     </row>
     <row r="287" spans="3:3">
-      <c r="C287" s="19"/>
+      <c r="C287" s="28"/>
     </row>
     <row r="288" spans="3:3">
-      <c r="C288" s="19"/>
+      <c r="C288" s="28"/>
     </row>
     <row r="289" spans="3:3">
-      <c r="C289" s="19"/>
+      <c r="C289" s="28"/>
     </row>
     <row r="290" spans="3:3">
-      <c r="C290" s="19"/>
+      <c r="C290" s="28"/>
     </row>
     <row r="291" spans="3:3">
-      <c r="C291" s="19"/>
+      <c r="C291" s="28"/>
     </row>
     <row r="292" spans="3:3">
-      <c r="C292" s="19"/>
+      <c r="C292" s="28"/>
     </row>
     <row r="293" spans="3:3">
-      <c r="C293" s="19"/>
+      <c r="C293" s="28"/>
     </row>
     <row r="294" spans="3:3">
-      <c r="C294" s="19"/>
+      <c r="C294" s="28"/>
     </row>
     <row r="295" spans="3:3">
-      <c r="C295" s="19"/>
+      <c r="C295" s="28"/>
     </row>
     <row r="296" spans="3:3">
-      <c r="C296" s="19"/>
+      <c r="C296" s="28"/>
     </row>
     <row r="297" spans="3:3">
-      <c r="C297" s="19"/>
+      <c r="C297" s="28"/>
     </row>
     <row r="298" spans="3:3">
-      <c r="C298" s="19"/>
+      <c r="C298" s="28"/>
     </row>
     <row r="299" spans="3:3">
-      <c r="C299" s="19"/>
+      <c r="C299" s="28"/>
     </row>
     <row r="300" spans="3:3">
-      <c r="C300" s="19"/>
+      <c r="C300" s="28"/>
     </row>
     <row r="301" spans="3:3">
-      <c r="C301" s="19"/>
+      <c r="C301" s="28"/>
     </row>
     <row r="302" spans="3:3">
-      <c r="C302" s="19"/>
+      <c r="C302" s="28"/>
     </row>
     <row r="303" spans="3:3">
-      <c r="C303" s="19"/>
+      <c r="C303" s="28"/>
     </row>
     <row r="304" spans="3:3">
-      <c r="C304" s="19"/>
+      <c r="C304" s="28"/>
     </row>
     <row r="305" spans="3:3">
-      <c r="C305" s="19"/>
+      <c r="C305" s="28"/>
     </row>
     <row r="306" spans="3:3">
-      <c r="C306" s="19"/>
+      <c r="C306" s="28"/>
     </row>
     <row r="307" spans="3:3">
-      <c r="C307" s="19"/>
+      <c r="C307" s="28"/>
     </row>
     <row r="308" spans="3:3">
-      <c r="C308" s="19"/>
+      <c r="C308" s="28"/>
     </row>
     <row r="309" spans="3:3">
-      <c r="C309" s="19"/>
+      <c r="C309" s="28"/>
     </row>
     <row r="310" spans="3:3">
-      <c r="C310" s="19"/>
+      <c r="C310" s="28"/>
     </row>
     <row r="311" spans="3:3">
-      <c r="C311" s="19"/>
+      <c r="C311" s="28"/>
     </row>
     <row r="312" spans="3:3">
-      <c r="C312" s="19"/>
+      <c r="C312" s="28"/>
     </row>
     <row r="313" spans="3:3">
-      <c r="C313" s="19"/>
+      <c r="C313" s="28"/>
     </row>
     <row r="314" spans="3:3">
-      <c r="C314" s="19"/>
+      <c r="C314" s="28"/>
     </row>
     <row r="315" spans="3:3">
-      <c r="C315" s="19"/>
+      <c r="C315" s="28"/>
     </row>
     <row r="316" spans="3:3">
-      <c r="C316" s="19"/>
+      <c r="C316" s="28"/>
     </row>
     <row r="317" spans="3:3">
-      <c r="C317" s="19"/>
+      <c r="C317" s="28"/>
     </row>
     <row r="318" spans="3:3">
-      <c r="C318" s="19"/>
+      <c r="C318" s="28"/>
     </row>
     <row r="319" spans="3:3">
-      <c r="C319" s="19"/>
+      <c r="C319" s="28"/>
     </row>
     <row r="320" spans="3:3">
-      <c r="C320" s="19"/>
+      <c r="C320" s="28"/>
     </row>
     <row r="321" spans="3:3">
-      <c r="C321" s="19"/>
+      <c r="C321" s="28"/>
     </row>
     <row r="322" spans="3:3">
-      <c r="C322" s="19"/>
+      <c r="C322" s="28"/>
     </row>
     <row r="323" spans="3:3">
-      <c r="C323" s="19"/>
+      <c r="C323" s="28"/>
     </row>
     <row r="324" spans="3:3">
-      <c r="C324" s="19"/>
+      <c r="C324" s="28"/>
     </row>
     <row r="325" spans="3:3">
-      <c r="C325" s="19"/>
+      <c r="C325" s="28"/>
     </row>
     <row r="326" spans="3:3">
-      <c r="C326" s="19"/>
+      <c r="C326" s="28"/>
     </row>
     <row r="327" spans="3:3">
-      <c r="C327" s="19"/>
+      <c r="C327" s="28"/>
     </row>
     <row r="328" spans="3:3">
-      <c r="C328" s="19"/>
+      <c r="C328" s="28"/>
     </row>
     <row r="329" spans="3:3">
-      <c r="C329" s="19"/>
+      <c r="C329" s="28"/>
     </row>
     <row r="330" spans="3:3">
-      <c r="C330" s="19"/>
+      <c r="C330" s="28"/>
     </row>
     <row r="331" spans="3:3">
-      <c r="C331" s="19"/>
+      <c r="C331" s="28"/>
     </row>
     <row r="332" spans="3:3">
-      <c r="C332" s="19"/>
+      <c r="C332" s="28"/>
     </row>
     <row r="333" spans="3:3">
-      <c r="C333" s="19"/>
+      <c r="C333" s="28"/>
     </row>
     <row r="334" spans="3:3">
-      <c r="C334" s="19"/>
+      <c r="C334" s="28"/>
     </row>
     <row r="335" spans="3:3">
-      <c r="C335" s="19"/>
+      <c r="C335" s="28"/>
     </row>
     <row r="336" spans="3:3">
-      <c r="C336" s="19"/>
+      <c r="C336" s="28"/>
     </row>
     <row r="337" spans="3:3">
-      <c r="C337" s="19"/>
+      <c r="C337" s="28"/>
     </row>
     <row r="338" spans="3:3">
-      <c r="C338" s="19"/>
+      <c r="C338" s="28"/>
     </row>
     <row r="339" spans="3:3">
-      <c r="C339" s="19"/>
+      <c r="C339" s="28"/>
     </row>
     <row r="340" spans="3:3">
-      <c r="C340" s="19"/>
+      <c r="C340" s="28"/>
     </row>
     <row r="341" spans="3:3">
-      <c r="C341" s="19"/>
+      <c r="C341" s="28"/>
     </row>
     <row r="342" spans="3:3">
-      <c r="C342" s="19"/>
+      <c r="C342" s="28"/>
     </row>
     <row r="343" spans="3:3">
-      <c r="C343" s="19"/>
+      <c r="C343" s="28"/>
     </row>
     <row r="344" spans="3:3">
-      <c r="C344" s="19"/>
+      <c r="C344" s="28"/>
     </row>
     <row r="345" spans="3:3">
-      <c r="C345" s="19"/>
+      <c r="C345" s="28"/>
     </row>
     <row r="346" spans="3:3">
-      <c r="C346" s="19"/>
+      <c r="C346" s="28"/>
     </row>
     <row r="347" spans="3:3">
-      <c r="C347" s="19"/>
+      <c r="C347" s="28"/>
     </row>
     <row r="348" spans="3:3">
-      <c r="C348" s="19"/>
+      <c r="C348" s="28"/>
     </row>
     <row r="349" spans="3:3">
-      <c r="C349" s="19"/>
+      <c r="C349" s="28"/>
     </row>
     <row r="350" spans="3:3">
-      <c r="C350" s="19"/>
+      <c r="C350" s="28"/>
     </row>
     <row r="351" spans="3:3">
-      <c r="C351" s="19"/>
+      <c r="C351" s="28"/>
     </row>
     <row r="352" spans="3:3">
-      <c r="C352" s="19"/>
+      <c r="C352" s="28"/>
     </row>
     <row r="353" spans="3:3">
-      <c r="C353" s="19"/>
+      <c r="C353" s="28"/>
     </row>
     <row r="354" spans="3:3">
-      <c r="C354" s="19"/>
+      <c r="C354" s="28"/>
     </row>
     <row r="355" spans="3:3">
-      <c r="C355" s="19"/>
+      <c r="C355" s="28"/>
     </row>
     <row r="356" spans="3:3">
-      <c r="C356" s="19"/>
+      <c r="C356" s="28"/>
     </row>
     <row r="357" spans="3:3">
-      <c r="C357" s="19"/>
+      <c r="C357" s="28"/>
     </row>
     <row r="358" spans="3:3">
-      <c r="C358" s="19"/>
+      <c r="C358" s="28"/>
     </row>
     <row r="359" spans="3:3">
-      <c r="C359" s="19"/>
+      <c r="C359" s="28"/>
     </row>
     <row r="360" spans="3:3">
-      <c r="C360" s="19"/>
+      <c r="C360" s="28"/>
     </row>
     <row r="361" spans="3:3">
-      <c r="C361" s="19"/>
+      <c r="C361" s="28"/>
     </row>
     <row r="362" spans="3:3">
-      <c r="C362" s="19"/>
+      <c r="C362" s="28"/>
     </row>
     <row r="363" spans="3:3">
-      <c r="C363" s="19"/>
+      <c r="C363" s="28"/>
     </row>
     <row r="364" spans="3:3">
-      <c r="C364" s="19"/>
+      <c r="C364" s="28"/>
     </row>
     <row r="365" spans="3:3">
-      <c r="C365" s="19"/>
+      <c r="C365" s="28"/>
     </row>
     <row r="366" spans="3:3">
-      <c r="C366" s="19"/>
+      <c r="C366" s="28"/>
     </row>
     <row r="367" spans="3:3">
-      <c r="C367" s="19"/>
+      <c r="C367" s="28"/>
     </row>
     <row r="368" spans="3:3">
-      <c r="C368" s="19"/>
+      <c r="C368" s="28"/>
     </row>
     <row r="369" spans="3:3">
-      <c r="C369" s="19"/>
+      <c r="C369" s="28"/>
     </row>
     <row r="370" spans="3:3">
-      <c r="C370" s="19"/>
+      <c r="C370" s="28"/>
     </row>
     <row r="371" spans="3:3">
-      <c r="C371" s="19"/>
+      <c r="C371" s="28"/>
     </row>
     <row r="372" spans="3:3">
-      <c r="C372" s="19"/>
+      <c r="C372" s="28"/>
     </row>
     <row r="373" spans="3:3">
-      <c r="C373" s="19"/>
+      <c r="C373" s="28"/>
     </row>
     <row r="374" spans="3:3">
-      <c r="C374" s="19"/>
+      <c r="C374" s="28"/>
     </row>
     <row r="375" spans="3:3">
-      <c r="C375" s="19"/>
+      <c r="C375" s="28"/>
     </row>
     <row r="376" spans="3:3">
-      <c r="C376" s="19"/>
+      <c r="C376" s="28"/>
     </row>
     <row r="377" spans="3:3">
-      <c r="C377" s="19"/>
+      <c r="C377" s="28"/>
     </row>
     <row r="378" spans="3:3">
-      <c r="C378" s="19"/>
+      <c r="C378" s="28"/>
     </row>
     <row r="379" spans="3:3">
-      <c r="C379" s="19"/>
+      <c r="C379" s="28"/>
     </row>
     <row r="380" spans="3:3">
-      <c r="C380" s="19"/>
+      <c r="C380" s="28"/>
     </row>
     <row r="381" spans="3:3">
-      <c r="C381" s="19"/>
+      <c r="C381" s="28"/>
     </row>
     <row r="382" spans="3:3">
-      <c r="C382" s="19"/>
+      <c r="C382" s="28"/>
     </row>
     <row r="383" spans="3:3">
-      <c r="C383" s="19"/>
+      <c r="C383" s="28"/>
     </row>
     <row r="384" spans="3:3">
-      <c r="C384" s="19"/>
+      <c r="C384" s="28"/>
     </row>
     <row r="385" spans="3:3">
-      <c r="C385" s="19"/>
+      <c r="C385" s="28"/>
     </row>
     <row r="386" spans="3:3">
-      <c r="C386" s="19"/>
+      <c r="C386" s="28"/>
     </row>
     <row r="387" spans="3:3">
-      <c r="C387" s="19"/>
+      <c r="C387" s="28"/>
     </row>
     <row r="388" spans="3:3">
-      <c r="C388" s="19"/>
+      <c r="C388" s="28"/>
     </row>
     <row r="389" spans="3:3">
-      <c r="C389" s="19"/>
+      <c r="C389" s="28"/>
     </row>
     <row r="390" spans="3:3">
-      <c r="C390" s="19"/>
+      <c r="C390" s="28"/>
     </row>
     <row r="391" spans="3:3">
-      <c r="C391" s="19"/>
+      <c r="C391" s="28"/>
     </row>
     <row r="392" spans="3:3">
-      <c r="C392" s="19"/>
+      <c r="C392" s="28"/>
     </row>
     <row r="393" spans="3:3">
-      <c r="C393" s="19"/>
+      <c r="C393" s="28"/>
     </row>
     <row r="394" spans="3:3">
-      <c r="C394" s="19"/>
+      <c r="C394" s="28"/>
     </row>
     <row r="395" spans="3:3">
-      <c r="C395" s="19"/>
+      <c r="C395" s="28"/>
     </row>
     <row r="396" spans="3:3">
-      <c r="C396" s="19"/>
+      <c r="C396" s="28"/>
     </row>
     <row r="397" spans="3:3">
-      <c r="C397" s="19"/>
+      <c r="C397" s="28"/>
     </row>
     <row r="398" spans="3:3">
-      <c r="C398" s="19"/>
+      <c r="C398" s="28"/>
     </row>
     <row r="399" spans="3:3">
-      <c r="C399" s="19"/>
+      <c r="C399" s="28"/>
     </row>
     <row r="400" spans="3:3">
-      <c r="C400" s="19"/>
+      <c r="C400" s="28"/>
     </row>
     <row r="401" spans="3:3">
-      <c r="C401" s="19"/>
+      <c r="C401" s="28"/>
     </row>
     <row r="402" spans="3:3">
-      <c r="C402" s="19"/>
+      <c r="C402" s="28"/>
     </row>
     <row r="403" spans="3:3">
-      <c r="C403" s="19"/>
+      <c r="C403" s="28"/>
     </row>
     <row r="404" spans="3:3">
-      <c r="C404" s="19"/>
+      <c r="C404" s="28"/>
     </row>
     <row r="405" spans="3:3">
-      <c r="C405" s="19"/>
+      <c r="C405" s="28"/>
     </row>
     <row r="406" spans="3:3">
-      <c r="C406" s="19"/>
+      <c r="C406" s="28"/>
     </row>
     <row r="407" spans="3:3">
-      <c r="C407" s="19"/>
+      <c r="C407" s="28"/>
     </row>
     <row r="408" spans="3:3">
-      <c r="C408" s="19"/>
+      <c r="C408" s="28"/>
     </row>
     <row r="409" spans="3:3">
-      <c r="C409" s="19"/>
+      <c r="C409" s="28"/>
     </row>
     <row r="410" spans="3:3">
-      <c r="C410" s="19"/>
+      <c r="C410" s="28"/>
     </row>
     <row r="411" spans="3:3">
-      <c r="C411" s="19"/>
+      <c r="C411" s="28"/>
     </row>
     <row r="412" spans="3:3">
-      <c r="C412" s="19"/>
+      <c r="C412" s="28"/>
     </row>
     <row r="413" spans="3:3">
-      <c r="C413" s="19"/>
+      <c r="C413" s="28"/>
     </row>
     <row r="414" spans="3:3">
-      <c r="C414" s="19"/>
+      <c r="C414" s="28"/>
     </row>
     <row r="415" spans="3:3">
-      <c r="C415" s="19"/>
+      <c r="C415" s="28"/>
     </row>
     <row r="416" spans="3:3">
-      <c r="C416" s="19"/>
+      <c r="C416" s="28"/>
     </row>
     <row r="417" spans="3:3">
-      <c r="C417" s="19"/>
+      <c r="C417" s="28"/>
     </row>
     <row r="418" spans="3:3">
-      <c r="C418" s="19"/>
+      <c r="C418" s="28"/>
     </row>
     <row r="419" spans="3:3">
-      <c r="C419" s="19"/>
+      <c r="C419" s="28"/>
     </row>
     <row r="420" spans="3:3">
-      <c r="C420" s="19"/>
+      <c r="C420" s="28"/>
     </row>
     <row r="421" spans="3:3">
-      <c r="C421" s="19"/>
+      <c r="C421" s="28"/>
     </row>
     <row r="422" spans="3:3">
-      <c r="C422" s="19"/>
+      <c r="C422" s="28"/>
     </row>
     <row r="423" spans="3:3">
-      <c r="C423" s="19"/>
+      <c r="C423" s="28"/>
     </row>
     <row r="424" spans="3:3">
-      <c r="C424" s="19"/>
+      <c r="C424" s="28"/>
     </row>
     <row r="425" spans="3:3">
-      <c r="C425" s="19"/>
+      <c r="C425" s="28"/>
     </row>
     <row r="426" spans="3:3">
-      <c r="C426" s="19"/>
+      <c r="C426" s="28"/>
     </row>
     <row r="434" spans="3:3">
-      <c r="C434" s="24"/>
+      <c r="C434" s="33"/>
     </row>
     <row r="435" spans="3:3">
-      <c r="C435" s="24"/>
+      <c r="C435" s="33"/>
     </row>
     <row r="436" spans="3:3">
-      <c r="C436" s="24"/>
+      <c r="C436" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3746,7 +4051,7 @@
   <sheetPr/>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3761,33 +4066,33 @@
   <sheetData>
     <row r="1" ht="14.25" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>108</v>
+        <v>157</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>109</v>
+        <v>158</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>110</v>
+        <v>159</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>111</v>
+        <v>160</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>112</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>114</v>
+        <v>163</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>115</v>
+        <v>164</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>116</v>
+        <v>165</v>
       </c>
       <c r="E2" s="4">
         <v>1</v>

</xml_diff>

<commit_message>
Fix in_migration and out_migration xml filenames (just storing in repo)
</commit_message>
<xml_diff>
--- a/src/main/resources/samples/extension-forms/xls/household_proxy_head_ext.xlsx
+++ b/src/main/resources/samples/extension-forms/xls/household_proxy_head_ext.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="166">
   <si>
     <t>type</t>
   </si>
@@ -525,8 +525,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
@@ -572,6 +572,14 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -582,37 +590,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -633,23 +610,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -665,14 +642,44 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -686,31 +693,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -761,7 +761,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -773,67 +887,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -845,49 +899,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -899,37 +917,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -954,15 +954,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1001,7 +992,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1035,6 +1026,15 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -1044,159 +1044,159 @@
   <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1248,10 +1248,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1687,11 +1683,11 @@
   <dimension ref="A1:V57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -1715,221 +1711,221 @@
     <col min="18" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" s="34" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
-      <c r="A1" s="38" t="s">
+    <row r="1" s="32" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="45" t="s">
+      <c r="J1" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="38" t="s">
+      <c r="K1" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="38" t="s">
+      <c r="M1" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="45" t="s">
+      <c r="N1" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="38" t="s">
+      <c r="O1" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="38" t="s">
+      <c r="P1" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="38" t="s">
+      <c r="Q1" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="38" t="s">
+      <c r="R1" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="38" t="s">
+      <c r="S1" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="38" t="s">
+      <c r="T1" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="38" t="s">
+      <c r="U1" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="38" t="s">
+      <c r="V1" s="36" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" s="35" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
-      <c r="A2" s="40" t="s">
+    <row r="2" s="33" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
+      <c r="A2" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="46" t="s">
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
-      <c r="U2" s="43"/>
-      <c r="V2" s="43"/>
-    </row>
-    <row r="3" s="35" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
-      <c r="A3" s="40" t="s">
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="41"/>
+      <c r="U2" s="41"/>
+      <c r="V2" s="41"/>
+    </row>
+    <row r="3" s="33" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
+      <c r="A3" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="46" t="s">
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="43"/>
-      <c r="R3" s="43"/>
-      <c r="S3" s="43"/>
-      <c r="T3" s="43"/>
-      <c r="U3" s="43"/>
-      <c r="V3" s="43"/>
-    </row>
-    <row r="4" s="35" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
-      <c r="A4" s="40" t="s">
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="41"/>
+      <c r="S3" s="41"/>
+      <c r="T3" s="41"/>
+      <c r="U3" s="41"/>
+      <c r="V3" s="41"/>
+    </row>
+    <row r="4" s="33" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
+      <c r="A4" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="46" t="s">
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="46"/>
-      <c r="O4" s="43"/>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="43"/>
-      <c r="R4" s="43"/>
-      <c r="S4" s="43"/>
-      <c r="T4" s="43"/>
-      <c r="U4" s="43"/>
-      <c r="V4" s="43"/>
-    </row>
-    <row r="5" s="36" customFormat="1" spans="1:14">
-      <c r="A5" s="36" t="s">
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="41"/>
+      <c r="Q4" s="41"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="41"/>
+      <c r="T4" s="41"/>
+      <c r="U4" s="41"/>
+      <c r="V4" s="41"/>
+    </row>
+    <row r="5" s="34" customFormat="1" spans="1:14">
+      <c r="A5" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="47" t="s">
+      <c r="J5" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="N5" s="47" t="s">
+      <c r="N5" s="45" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" s="36" customFormat="1" spans="1:14">
-      <c r="A6" s="36" t="s">
+    <row r="6" s="34" customFormat="1" spans="1:14">
+      <c r="A6" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="40" t="s">
         <v>32</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="47" t="s">
+      <c r="J6" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="N6" s="47" t="s">
+      <c r="N6" s="45" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" s="36" customFormat="1" spans="1:14">
-      <c r="A7" s="36" t="s">
+    <row r="7" s="34" customFormat="1" spans="1:14">
+      <c r="A7" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="34" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -1938,18 +1934,18 @@
       <c r="D7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="J7" s="47" t="s">
+      <c r="J7" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="N7" s="47" t="s">
+      <c r="N7" s="45" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" s="36" customFormat="1" spans="1:14">
-      <c r="A8" s="36" t="s">
+    <row r="8" s="34" customFormat="1" spans="1:14">
+      <c r="A8" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="34" t="s">
         <v>37</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -1958,18 +1954,18 @@
       <c r="D8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="47" t="s">
+      <c r="J8" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="N8" s="47" t="s">
+      <c r="N8" s="45" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" s="36" customFormat="1" customHeight="1" spans="1:14">
-      <c r="A9" s="36" t="s">
+    <row r="9" s="34" customFormat="1" customHeight="1" spans="1:14">
+      <c r="A9" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="34" t="s">
         <v>41</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -1978,18 +1974,18 @@
       <c r="D9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="47" t="s">
+      <c r="J9" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="N9" s="47" t="s">
+      <c r="N9" s="45" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" s="36" customFormat="1" customHeight="1" spans="1:14">
-      <c r="A10" s="36" t="s">
+    <row r="10" s="34" customFormat="1" customHeight="1" spans="1:14">
+      <c r="A10" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="34" t="s">
         <v>44</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -1998,18 +1994,16 @@
       <c r="D10" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="J10" s="47" t="s">
+      <c r="J10" s="45"/>
+      <c r="N10" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="N10" s="47" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" s="36" customFormat="1" spans="1:14">
-      <c r="A11" s="36" t="s">
+    </row>
+    <row r="11" s="34" customFormat="1" spans="1:14">
+      <c r="A11" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="34" t="s">
         <v>47</v>
       </c>
       <c r="C11" s="7" t="s">
@@ -2018,18 +2012,18 @@
       <c r="D11" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="J11" s="47" t="s">
+      <c r="J11" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="N11" s="47" t="s">
+      <c r="N11" s="45" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" s="36" customFormat="1" spans="1:14">
-      <c r="A12" s="36" t="s">
+    <row r="12" s="34" customFormat="1" spans="1:14">
+      <c r="A12" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="34" t="s">
         <v>51</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -2038,225 +2032,225 @@
       <c r="D12" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J12" s="47" t="s">
+      <c r="J12" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="N12" s="47" t="s">
+      <c r="N12" s="45" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" s="37" customFormat="1" spans="1:14">
-      <c r="A13" s="37" t="s">
+    <row r="13" s="35" customFormat="1" spans="1:14">
+      <c r="A13" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="J13" s="48"/>
-      <c r="N13" s="48"/>
-    </row>
-    <row r="14" s="37" customFormat="1" customHeight="1" spans="1:14">
-      <c r="A14" s="37" t="s">
+      <c r="J13" s="46"/>
+      <c r="N13" s="46"/>
+    </row>
+    <row r="14" s="35" customFormat="1" customHeight="1" spans="1:14">
+      <c r="A14" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="37" t="s">
+      <c r="D14" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="J14" s="48"/>
-      <c r="N14" s="48"/>
-    </row>
-    <row r="15" s="36" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J15" s="47"/>
-      <c r="N15" s="47"/>
-    </row>
-    <row r="16" s="36" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J16" s="47"/>
-      <c r="N16" s="47"/>
-    </row>
-    <row r="17" s="36" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J17" s="47"/>
-      <c r="N17" s="47"/>
-    </row>
-    <row r="18" s="36" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J18" s="47"/>
-      <c r="N18" s="47"/>
-    </row>
-    <row r="19" s="36" customFormat="1" spans="10:14">
-      <c r="J19" s="47"/>
-      <c r="N19" s="47"/>
-    </row>
-    <row r="20" s="36" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J20" s="47"/>
-      <c r="N20" s="47"/>
-    </row>
-    <row r="21" s="36" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J21" s="47"/>
-      <c r="N21" s="47"/>
-    </row>
-    <row r="22" s="36" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J22" s="47"/>
-      <c r="N22" s="47"/>
-    </row>
-    <row r="23" s="36" customFormat="1" spans="10:14">
-      <c r="J23" s="47"/>
-      <c r="N23" s="47"/>
-    </row>
-    <row r="24" s="36" customFormat="1" spans="10:14">
-      <c r="J24" s="47"/>
-      <c r="N24" s="47"/>
-    </row>
-    <row r="25" s="36" customFormat="1" spans="10:14">
-      <c r="J25" s="47"/>
-      <c r="N25" s="47"/>
-    </row>
-    <row r="26" s="36" customFormat="1" ht="15.75" customHeight="1" spans="10:14">
-      <c r="J26" s="47"/>
-      <c r="N26" s="47"/>
-    </row>
-    <row r="27" s="36" customFormat="1" ht="13.5" customHeight="1" spans="10:14">
-      <c r="J27" s="47"/>
-      <c r="N27" s="47"/>
-    </row>
-    <row r="28" s="36" customFormat="1" spans="10:14">
-      <c r="J28" s="47"/>
-      <c r="N28" s="47"/>
-    </row>
-    <row r="29" s="36" customFormat="1" spans="10:14">
-      <c r="J29" s="47"/>
-      <c r="N29" s="47"/>
-    </row>
-    <row r="30" s="36" customFormat="1" spans="10:14">
-      <c r="J30" s="47"/>
-      <c r="N30" s="47"/>
-    </row>
-    <row r="31" s="36" customFormat="1" ht="13.5" customHeight="1" spans="10:14">
-      <c r="J31" s="47"/>
-      <c r="N31" s="47"/>
-    </row>
-    <row r="32" s="36" customFormat="1" spans="10:14">
-      <c r="J32" s="47"/>
-      <c r="N32" s="47"/>
-    </row>
-    <row r="33" s="36" customFormat="1" spans="10:14">
-      <c r="J33" s="47"/>
-      <c r="N33" s="47"/>
-    </row>
-    <row r="34" s="36" customFormat="1" spans="10:14">
-      <c r="J34" s="47"/>
-      <c r="N34" s="47"/>
-    </row>
-    <row r="35" s="36" customFormat="1" spans="10:14">
-      <c r="J35" s="47"/>
-      <c r="N35" s="47"/>
-    </row>
-    <row r="36" s="36" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J36" s="47"/>
-      <c r="N36" s="47"/>
-    </row>
-    <row r="37" s="36" customFormat="1" ht="12" customHeight="1" spans="10:14">
-      <c r="J37" s="47"/>
-      <c r="N37" s="47"/>
-    </row>
-    <row r="38" s="36" customFormat="1" spans="10:14">
-      <c r="J38" s="47"/>
-      <c r="N38" s="47"/>
-    </row>
-    <row r="39" s="36" customFormat="1" spans="10:14">
-      <c r="J39" s="47"/>
-      <c r="N39" s="47"/>
-    </row>
-    <row r="40" s="36" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J40" s="47"/>
-      <c r="N40" s="47"/>
-    </row>
-    <row r="41" s="36" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J41" s="47"/>
-      <c r="N41" s="47"/>
-    </row>
-    <row r="42" s="36" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J42" s="47"/>
-      <c r="N42" s="47"/>
-    </row>
-    <row r="43" s="36" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J43" s="47"/>
-      <c r="N43" s="47"/>
-    </row>
-    <row r="44" s="36" customFormat="1" spans="10:14">
-      <c r="J44" s="47"/>
-      <c r="N44" s="47"/>
-    </row>
-    <row r="45" s="36" customFormat="1" spans="10:14">
-      <c r="J45" s="47"/>
-      <c r="N45" s="47"/>
-    </row>
-    <row r="46" s="36" customFormat="1" spans="10:14">
-      <c r="J46" s="47"/>
-      <c r="N46" s="47"/>
-    </row>
-    <row r="47" s="36" customFormat="1" spans="10:14">
-      <c r="J47" s="47"/>
-      <c r="N47" s="47"/>
-    </row>
-    <row r="48" s="36" customFormat="1" spans="10:14">
-      <c r="J48" s="47"/>
-      <c r="N48" s="47"/>
-    </row>
-    <row r="49" s="36" customFormat="1" spans="10:14">
-      <c r="J49" s="47"/>
-      <c r="N49" s="47"/>
-    </row>
-    <row r="50" s="36" customFormat="1" spans="10:14">
-      <c r="J50" s="47"/>
-      <c r="N50" s="47"/>
-    </row>
-    <row r="51" s="36" customFormat="1" spans="10:14">
-      <c r="J51" s="47"/>
-      <c r="N51" s="47"/>
-    </row>
-    <row r="52" s="36" customFormat="1" spans="10:14">
-      <c r="J52" s="47"/>
-      <c r="N52" s="47"/>
-    </row>
-    <row r="53" s="36" customFormat="1" spans="10:14">
-      <c r="J53" s="47"/>
-      <c r="N53" s="47"/>
-    </row>
-    <row r="54" s="36" customFormat="1" spans="10:14">
-      <c r="J54" s="47"/>
-      <c r="N54" s="47"/>
-    </row>
-    <row r="55" s="36" customFormat="1" spans="10:14">
-      <c r="J55" s="47"/>
-      <c r="N55" s="47"/>
-    </row>
-    <row r="56" s="36" customFormat="1" spans="10:14">
-      <c r="J56" s="47"/>
-      <c r="N56" s="47"/>
+      <c r="J14" s="46"/>
+      <c r="N14" s="46"/>
+    </row>
+    <row r="15" s="34" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J15" s="45"/>
+      <c r="N15" s="45"/>
+    </row>
+    <row r="16" s="34" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J16" s="45"/>
+      <c r="N16" s="45"/>
+    </row>
+    <row r="17" s="34" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J17" s="45"/>
+      <c r="N17" s="45"/>
+    </row>
+    <row r="18" s="34" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J18" s="45"/>
+      <c r="N18" s="45"/>
+    </row>
+    <row r="19" s="34" customFormat="1" spans="10:14">
+      <c r="J19" s="45"/>
+      <c r="N19" s="45"/>
+    </row>
+    <row r="20" s="34" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J20" s="45"/>
+      <c r="N20" s="45"/>
+    </row>
+    <row r="21" s="34" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J21" s="45"/>
+      <c r="N21" s="45"/>
+    </row>
+    <row r="22" s="34" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J22" s="45"/>
+      <c r="N22" s="45"/>
+    </row>
+    <row r="23" s="34" customFormat="1" spans="10:14">
+      <c r="J23" s="45"/>
+      <c r="N23" s="45"/>
+    </row>
+    <row r="24" s="34" customFormat="1" spans="10:14">
+      <c r="J24" s="45"/>
+      <c r="N24" s="45"/>
+    </row>
+    <row r="25" s="34" customFormat="1" spans="10:14">
+      <c r="J25" s="45"/>
+      <c r="N25" s="45"/>
+    </row>
+    <row r="26" s="34" customFormat="1" ht="15.75" customHeight="1" spans="10:14">
+      <c r="J26" s="45"/>
+      <c r="N26" s="45"/>
+    </row>
+    <row r="27" s="34" customFormat="1" ht="13.5" customHeight="1" spans="10:14">
+      <c r="J27" s="45"/>
+      <c r="N27" s="45"/>
+    </row>
+    <row r="28" s="34" customFormat="1" spans="10:14">
+      <c r="J28" s="45"/>
+      <c r="N28" s="45"/>
+    </row>
+    <row r="29" s="34" customFormat="1" spans="10:14">
+      <c r="J29" s="45"/>
+      <c r="N29" s="45"/>
+    </row>
+    <row r="30" s="34" customFormat="1" spans="10:14">
+      <c r="J30" s="45"/>
+      <c r="N30" s="45"/>
+    </row>
+    <row r="31" s="34" customFormat="1" ht="13.5" customHeight="1" spans="10:14">
+      <c r="J31" s="45"/>
+      <c r="N31" s="45"/>
+    </row>
+    <row r="32" s="34" customFormat="1" spans="10:14">
+      <c r="J32" s="45"/>
+      <c r="N32" s="45"/>
+    </row>
+    <row r="33" s="34" customFormat="1" spans="10:14">
+      <c r="J33" s="45"/>
+      <c r="N33" s="45"/>
+    </row>
+    <row r="34" s="34" customFormat="1" spans="10:14">
+      <c r="J34" s="45"/>
+      <c r="N34" s="45"/>
+    </row>
+    <row r="35" s="34" customFormat="1" spans="10:14">
+      <c r="J35" s="45"/>
+      <c r="N35" s="45"/>
+    </row>
+    <row r="36" s="34" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J36" s="45"/>
+      <c r="N36" s="45"/>
+    </row>
+    <row r="37" s="34" customFormat="1" ht="12" customHeight="1" spans="10:14">
+      <c r="J37" s="45"/>
+      <c r="N37" s="45"/>
+    </row>
+    <row r="38" s="34" customFormat="1" spans="10:14">
+      <c r="J38" s="45"/>
+      <c r="N38" s="45"/>
+    </row>
+    <row r="39" s="34" customFormat="1" spans="10:14">
+      <c r="J39" s="45"/>
+      <c r="N39" s="45"/>
+    </row>
+    <row r="40" s="34" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J40" s="45"/>
+      <c r="N40" s="45"/>
+    </row>
+    <row r="41" s="34" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J41" s="45"/>
+      <c r="N41" s="45"/>
+    </row>
+    <row r="42" s="34" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J42" s="45"/>
+      <c r="N42" s="45"/>
+    </row>
+    <row r="43" s="34" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J43" s="45"/>
+      <c r="N43" s="45"/>
+    </row>
+    <row r="44" s="34" customFormat="1" spans="10:14">
+      <c r="J44" s="45"/>
+      <c r="N44" s="45"/>
+    </row>
+    <row r="45" s="34" customFormat="1" spans="10:14">
+      <c r="J45" s="45"/>
+      <c r="N45" s="45"/>
+    </row>
+    <row r="46" s="34" customFormat="1" spans="10:14">
+      <c r="J46" s="45"/>
+      <c r="N46" s="45"/>
+    </row>
+    <row r="47" s="34" customFormat="1" spans="10:14">
+      <c r="J47" s="45"/>
+      <c r="N47" s="45"/>
+    </row>
+    <row r="48" s="34" customFormat="1" spans="10:14">
+      <c r="J48" s="45"/>
+      <c r="N48" s="45"/>
+    </row>
+    <row r="49" s="34" customFormat="1" spans="10:14">
+      <c r="J49" s="45"/>
+      <c r="N49" s="45"/>
+    </row>
+    <row r="50" s="34" customFormat="1" spans="10:14">
+      <c r="J50" s="45"/>
+      <c r="N50" s="45"/>
+    </row>
+    <row r="51" s="34" customFormat="1" spans="10:14">
+      <c r="J51" s="45"/>
+      <c r="N51" s="45"/>
+    </row>
+    <row r="52" s="34" customFormat="1" spans="10:14">
+      <c r="J52" s="45"/>
+      <c r="N52" s="45"/>
+    </row>
+    <row r="53" s="34" customFormat="1" spans="10:14">
+      <c r="J53" s="45"/>
+      <c r="N53" s="45"/>
+    </row>
+    <row r="54" s="34" customFormat="1" spans="10:14">
+      <c r="J54" s="45"/>
+      <c r="N54" s="45"/>
+    </row>
+    <row r="55" s="34" customFormat="1" spans="10:14">
+      <c r="J55" s="45"/>
+      <c r="N55" s="45"/>
+    </row>
+    <row r="56" s="34" customFormat="1" spans="10:14">
+      <c r="J56" s="45"/>
+      <c r="N56" s="45"/>
     </row>
     <row r="57" spans="1:11">
-      <c r="A57" s="36"/>
-      <c r="B57" s="36"/>
-      <c r="C57" s="36"/>
-      <c r="D57" s="36"/>
-      <c r="E57" s="36"/>
-      <c r="F57" s="36"/>
-      <c r="G57" s="36"/>
-      <c r="H57" s="36"/>
-      <c r="I57" s="36"/>
-      <c r="J57" s="47"/>
-      <c r="K57" s="36"/>
+      <c r="A57" s="34"/>
+      <c r="B57" s="34"/>
+      <c r="C57" s="34"/>
+      <c r="D57" s="34"/>
+      <c r="E57" s="34"/>
+      <c r="F57" s="34"/>
+      <c r="G57" s="34"/>
+      <c r="H57" s="34"/>
+      <c r="I57" s="34"/>
+      <c r="J57" s="45"/>
+      <c r="K57" s="34"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -2526,7 +2520,7 @@
       <c r="C17" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="7" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2534,13 +2528,13 @@
       <c r="A18" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="7" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2548,181 +2542,181 @@
       <c r="A19" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="7" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D20" s="24" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="D21" s="26" t="s">
+      <c r="D21" s="24" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="D22" s="26" t="s">
+      <c r="D22" s="24" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="D23" s="24" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="D24" s="26" t="s">
+      <c r="D24" s="24" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="D25" s="26" t="s">
+      <c r="D25" s="24" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="D26" s="26" t="s">
+      <c r="D26" s="24" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="D27" s="26" t="s">
+      <c r="D27" s="24" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="D28" s="26" t="s">
+      <c r="D28" s="24" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="D29" s="26" t="s">
+      <c r="D29" s="24" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="C30" s="25" t="s">
+      <c r="C30" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="D30" s="26" t="s">
+      <c r="D30" s="24" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="D31" s="26" t="s">
+      <c r="D31" s="24" t="s">
         <v>156</v>
       </c>
     </row>
@@ -2874,17 +2868,17 @@
     <row r="61" ht="15" spans="1:3">
       <c r="A61" s="17"/>
       <c r="B61" s="17"/>
-      <c r="C61" s="27"/>
+      <c r="C61" s="25"/>
     </row>
     <row r="62" ht="15" spans="1:3">
       <c r="A62" s="17"/>
       <c r="B62" s="17"/>
-      <c r="C62" s="27"/>
+      <c r="C62" s="25"/>
     </row>
     <row r="63" ht="15" spans="1:3">
       <c r="A63" s="17"/>
       <c r="B63" s="17"/>
-      <c r="C63" s="27"/>
+      <c r="C63" s="25"/>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="17"/>
@@ -3110,44 +3104,44 @@
       <c r="A108" s="17"/>
       <c r="B108" s="17"/>
       <c r="C108" s="6"/>
-      <c r="D108" s="28"/>
+      <c r="D108" s="26"/>
       <c r="E108"/>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="17"/>
       <c r="B109" s="17"/>
       <c r="C109" s="6"/>
-      <c r="D109" s="28"/>
+      <c r="D109" s="26"/>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="17"/>
       <c r="B110" s="17"/>
       <c r="C110" s="6"/>
-      <c r="D110" s="28"/>
+      <c r="D110" s="26"/>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="17"/>
       <c r="B111" s="17"/>
       <c r="C111" s="6"/>
-      <c r="D111" s="28"/>
+      <c r="D111" s="26"/>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="17"/>
       <c r="B112" s="17"/>
       <c r="C112" s="6"/>
-      <c r="D112" s="28"/>
+      <c r="D112" s="26"/>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="17"/>
       <c r="B113" s="17"/>
       <c r="C113" s="6"/>
-      <c r="D113" s="28"/>
+      <c r="D113" s="26"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="17"/>
       <c r="B114" s="17"/>
       <c r="C114" s="6"/>
-      <c r="D114" s="28"/>
+      <c r="D114" s="26"/>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" s="17"/>
@@ -3215,247 +3209,247 @@
       <c r="C127" s="6"/>
     </row>
     <row r="128" spans="3:3">
-      <c r="C128" s="29"/>
+      <c r="C128" s="27"/>
     </row>
     <row r="129" spans="3:3">
-      <c r="C129" s="29"/>
+      <c r="C129" s="27"/>
     </row>
     <row r="130" spans="3:3">
-      <c r="C130" s="29"/>
+      <c r="C130" s="27"/>
     </row>
     <row r="131" spans="3:3">
-      <c r="C131" s="29"/>
+      <c r="C131" s="27"/>
     </row>
     <row r="132" spans="3:3">
-      <c r="C132" s="29"/>
+      <c r="C132" s="27"/>
     </row>
     <row r="133" spans="3:3">
-      <c r="C133" s="29"/>
+      <c r="C133" s="27"/>
     </row>
     <row r="134" spans="3:3">
       <c r="C134" s="6"/>
     </row>
     <row r="135" spans="3:3">
-      <c r="C135" s="29"/>
+      <c r="C135" s="27"/>
     </row>
     <row r="136" spans="3:3">
-      <c r="C136" s="29"/>
+      <c r="C136" s="27"/>
     </row>
     <row r="137" spans="3:3">
-      <c r="C137" s="29"/>
+      <c r="C137" s="27"/>
     </row>
     <row r="138" spans="3:3">
-      <c r="C138" s="29"/>
+      <c r="C138" s="27"/>
     </row>
     <row r="139" spans="3:3">
-      <c r="C139" s="29"/>
+      <c r="C139" s="27"/>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="3"/>
-      <c r="C140" s="30"/>
+      <c r="C140" s="28"/>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="3"/>
-      <c r="C141" s="30"/>
+      <c r="C141" s="28"/>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" s="3"/>
-      <c r="C142" s="30"/>
+      <c r="C142" s="28"/>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="3"/>
-      <c r="C143" s="30"/>
+      <c r="C143" s="28"/>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="3"/>
-      <c r="C144" s="30"/>
+      <c r="C144" s="28"/>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" s="3"/>
-      <c r="C145" s="30"/>
+      <c r="C145" s="28"/>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="3"/>
-      <c r="C146" s="30"/>
+      <c r="C146" s="28"/>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="3"/>
-      <c r="C147" s="30"/>
+      <c r="C147" s="28"/>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" s="3"/>
-      <c r="C148" s="30"/>
+      <c r="C148" s="28"/>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="3"/>
-      <c r="C149" s="30"/>
+      <c r="C149" s="28"/>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" s="3"/>
-      <c r="C150" s="30"/>
+      <c r="C150" s="28"/>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" s="3"/>
-      <c r="C151" s="30"/>
+      <c r="C151" s="28"/>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" s="3"/>
-      <c r="C152" s="30"/>
+      <c r="C152" s="28"/>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" s="3"/>
-      <c r="C153" s="30"/>
+      <c r="C153" s="28"/>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" s="3"/>
-      <c r="C154" s="30"/>
+      <c r="C154" s="28"/>
     </row>
     <row r="155" spans="3:4">
-      <c r="C155" s="29"/>
-      <c r="D155" s="29"/>
+      <c r="C155" s="27"/>
+      <c r="D155" s="27"/>
     </row>
     <row r="156" spans="3:4">
-      <c r="C156" s="29"/>
-      <c r="D156" s="29"/>
+      <c r="C156" s="27"/>
+      <c r="D156" s="27"/>
     </row>
     <row r="157" spans="3:4">
-      <c r="C157" s="29"/>
-      <c r="D157" s="29"/>
+      <c r="C157" s="27"/>
+      <c r="D157" s="27"/>
     </row>
     <row r="158" spans="3:4">
-      <c r="C158" s="29"/>
-      <c r="D158" s="29"/>
+      <c r="C158" s="27"/>
+      <c r="D158" s="27"/>
     </row>
     <row r="159" spans="3:4">
-      <c r="C159" s="29"/>
-      <c r="D159" s="29"/>
+      <c r="C159" s="27"/>
+      <c r="D159" s="27"/>
     </row>
     <row r="160" spans="3:4">
-      <c r="C160" s="29"/>
-      <c r="D160" s="29"/>
+      <c r="C160" s="27"/>
+      <c r="D160" s="27"/>
     </row>
     <row r="161" spans="3:4">
-      <c r="C161" s="29"/>
-      <c r="D161" s="29"/>
+      <c r="C161" s="27"/>
+      <c r="D161" s="27"/>
     </row>
     <row r="162" spans="3:4">
-      <c r="C162" s="29"/>
-      <c r="D162" s="29"/>
+      <c r="C162" s="27"/>
+      <c r="D162" s="27"/>
     </row>
     <row r="163" spans="3:4">
       <c r="C163" s="6"/>
       <c r="D163" s="6"/>
     </row>
     <row r="164" spans="3:3">
-      <c r="C164" s="29"/>
+      <c r="C164" s="27"/>
     </row>
     <row r="165" spans="3:3">
-      <c r="C165" s="29"/>
+      <c r="C165" s="27"/>
     </row>
     <row r="166" spans="3:3">
-      <c r="C166" s="29"/>
+      <c r="C166" s="27"/>
     </row>
     <row r="167" spans="3:3">
-      <c r="C167" s="29"/>
+      <c r="C167" s="27"/>
     </row>
     <row r="168" spans="3:3">
-      <c r="C168" s="29"/>
+      <c r="C168" s="27"/>
     </row>
     <row r="169" spans="3:3">
-      <c r="C169" s="29"/>
+      <c r="C169" s="27"/>
     </row>
     <row r="170" spans="3:3">
-      <c r="C170" s="29"/>
+      <c r="C170" s="27"/>
     </row>
     <row r="171" spans="3:3">
-      <c r="C171" s="29"/>
+      <c r="C171" s="27"/>
     </row>
     <row r="172" spans="3:3">
-      <c r="C172" s="29"/>
+      <c r="C172" s="27"/>
     </row>
     <row r="173" spans="3:3">
-      <c r="C173" s="29"/>
+      <c r="C173" s="27"/>
     </row>
     <row r="174" spans="3:3">
-      <c r="C174" s="29"/>
+      <c r="C174" s="27"/>
     </row>
     <row r="175" spans="3:3">
-      <c r="C175" s="29"/>
+      <c r="C175" s="27"/>
     </row>
     <row r="176" spans="3:3">
-      <c r="C176" s="29"/>
+      <c r="C176" s="27"/>
     </row>
     <row r="177" spans="3:3">
-      <c r="C177" s="29"/>
+      <c r="C177" s="27"/>
     </row>
     <row r="178" spans="3:3">
-      <c r="C178" s="29"/>
+      <c r="C178" s="27"/>
     </row>
     <row r="195" spans="3:3">
-      <c r="C195" s="29"/>
+      <c r="C195" s="27"/>
     </row>
     <row r="196" spans="3:3">
-      <c r="C196" s="29"/>
+      <c r="C196" s="27"/>
     </row>
     <row r="197" spans="3:3">
-      <c r="C197" s="29"/>
+      <c r="C197" s="27"/>
     </row>
     <row r="198" spans="3:3">
-      <c r="C198" s="29"/>
+      <c r="C198" s="27"/>
     </row>
     <row r="199" spans="3:3">
-      <c r="C199" s="29"/>
+      <c r="C199" s="27"/>
     </row>
     <row r="200" spans="3:3">
-      <c r="C200" s="29"/>
+      <c r="C200" s="27"/>
     </row>
     <row r="201" spans="3:3">
-      <c r="C201" s="29"/>
+      <c r="C201" s="27"/>
     </row>
     <row r="202" spans="3:3">
-      <c r="C202" s="29"/>
+      <c r="C202" s="27"/>
     </row>
     <row r="203" spans="3:3">
-      <c r="C203" s="29"/>
+      <c r="C203" s="27"/>
     </row>
     <row r="204" spans="3:3">
-      <c r="C204" s="29"/>
+      <c r="C204" s="27"/>
     </row>
     <row r="205" spans="3:3">
-      <c r="C205" s="29"/>
+      <c r="C205" s="27"/>
     </row>
     <row r="206" spans="3:3">
-      <c r="C206" s="29"/>
+      <c r="C206" s="27"/>
     </row>
     <row r="207" spans="3:3">
-      <c r="C207" s="29"/>
+      <c r="C207" s="27"/>
     </row>
     <row r="208" spans="3:3">
-      <c r="C208" s="29"/>
+      <c r="C208" s="27"/>
     </row>
     <row r="209" spans="3:3">
-      <c r="C209" s="29"/>
+      <c r="C209" s="27"/>
     </row>
     <row r="210" spans="3:3">
-      <c r="C210" s="29"/>
+      <c r="C210" s="27"/>
     </row>
     <row r="211" spans="3:3">
-      <c r="C211" s="29"/>
+      <c r="C211" s="27"/>
     </row>
     <row r="212" spans="3:3">
-      <c r="C212" s="29"/>
+      <c r="C212" s="27"/>
     </row>
     <row r="213" spans="3:3">
-      <c r="C213" s="29"/>
+      <c r="C213" s="27"/>
     </row>
     <row r="225" spans="3:3">
-      <c r="C225" s="31"/>
+      <c r="C225" s="29"/>
     </row>
     <row r="226" spans="3:3">
-      <c r="C226" s="31"/>
+      <c r="C226" s="29"/>
     </row>
     <row r="227" spans="3:3">
-      <c r="C227" s="32"/>
+      <c r="C227" s="30"/>
     </row>
     <row r="236" spans="3:3">
       <c r="C236" s="4"/>
@@ -3557,487 +3551,487 @@
       <c r="C268" s="4"/>
     </row>
     <row r="269" spans="3:3">
-      <c r="C269" s="28"/>
+      <c r="C269" s="26"/>
     </row>
     <row r="270" spans="3:3">
-      <c r="C270" s="28"/>
+      <c r="C270" s="26"/>
     </row>
     <row r="271" spans="3:3">
-      <c r="C271" s="28"/>
+      <c r="C271" s="26"/>
     </row>
     <row r="272" spans="3:3">
-      <c r="C272" s="28"/>
+      <c r="C272" s="26"/>
     </row>
     <row r="273" spans="3:3">
-      <c r="C273" s="28"/>
+      <c r="C273" s="26"/>
     </row>
     <row r="274" spans="3:3">
-      <c r="C274" s="28"/>
+      <c r="C274" s="26"/>
     </row>
     <row r="275" spans="3:3">
-      <c r="C275" s="28"/>
+      <c r="C275" s="26"/>
     </row>
     <row r="276" spans="3:3">
-      <c r="C276" s="28"/>
+      <c r="C276" s="26"/>
     </row>
     <row r="277" spans="3:3">
-      <c r="C277" s="28"/>
+      <c r="C277" s="26"/>
     </row>
     <row r="278" spans="3:3">
-      <c r="C278" s="28"/>
+      <c r="C278" s="26"/>
     </row>
     <row r="279" spans="3:3">
-      <c r="C279" s="28"/>
+      <c r="C279" s="26"/>
     </row>
     <row r="280" spans="3:3">
-      <c r="C280" s="28"/>
+      <c r="C280" s="26"/>
     </row>
     <row r="281" spans="3:3">
-      <c r="C281" s="28"/>
+      <c r="C281" s="26"/>
     </row>
     <row r="282" spans="3:3">
-      <c r="C282" s="28"/>
+      <c r="C282" s="26"/>
     </row>
     <row r="283" spans="3:3">
-      <c r="C283" s="28"/>
+      <c r="C283" s="26"/>
     </row>
     <row r="284" spans="3:3">
-      <c r="C284" s="28"/>
+      <c r="C284" s="26"/>
     </row>
     <row r="285" spans="3:3">
-      <c r="C285" s="28"/>
+      <c r="C285" s="26"/>
     </row>
     <row r="286" spans="3:3">
-      <c r="C286" s="28"/>
+      <c r="C286" s="26"/>
     </row>
     <row r="287" spans="3:3">
-      <c r="C287" s="28"/>
+      <c r="C287" s="26"/>
     </row>
     <row r="288" spans="3:3">
-      <c r="C288" s="28"/>
+      <c r="C288" s="26"/>
     </row>
     <row r="289" spans="3:3">
-      <c r="C289" s="28"/>
+      <c r="C289" s="26"/>
     </row>
     <row r="290" spans="3:3">
-      <c r="C290" s="28"/>
+      <c r="C290" s="26"/>
     </row>
     <row r="291" spans="3:3">
-      <c r="C291" s="28"/>
+      <c r="C291" s="26"/>
     </row>
     <row r="292" spans="3:3">
-      <c r="C292" s="28"/>
+      <c r="C292" s="26"/>
     </row>
     <row r="293" spans="3:3">
-      <c r="C293" s="28"/>
+      <c r="C293" s="26"/>
     </row>
     <row r="294" spans="3:3">
-      <c r="C294" s="28"/>
+      <c r="C294" s="26"/>
     </row>
     <row r="295" spans="3:3">
-      <c r="C295" s="28"/>
+      <c r="C295" s="26"/>
     </row>
     <row r="296" spans="3:3">
-      <c r="C296" s="28"/>
+      <c r="C296" s="26"/>
     </row>
     <row r="297" spans="3:3">
-      <c r="C297" s="28"/>
+      <c r="C297" s="26"/>
     </row>
     <row r="298" spans="3:3">
-      <c r="C298" s="28"/>
+      <c r="C298" s="26"/>
     </row>
     <row r="299" spans="3:3">
-      <c r="C299" s="28"/>
+      <c r="C299" s="26"/>
     </row>
     <row r="300" spans="3:3">
-      <c r="C300" s="28"/>
+      <c r="C300" s="26"/>
     </row>
     <row r="301" spans="3:3">
-      <c r="C301" s="28"/>
+      <c r="C301" s="26"/>
     </row>
     <row r="302" spans="3:3">
-      <c r="C302" s="28"/>
+      <c r="C302" s="26"/>
     </row>
     <row r="303" spans="3:3">
-      <c r="C303" s="28"/>
+      <c r="C303" s="26"/>
     </row>
     <row r="304" spans="3:3">
-      <c r="C304" s="28"/>
+      <c r="C304" s="26"/>
     </row>
     <row r="305" spans="3:3">
-      <c r="C305" s="28"/>
+      <c r="C305" s="26"/>
     </row>
     <row r="306" spans="3:3">
-      <c r="C306" s="28"/>
+      <c r="C306" s="26"/>
     </row>
     <row r="307" spans="3:3">
-      <c r="C307" s="28"/>
+      <c r="C307" s="26"/>
     </row>
     <row r="308" spans="3:3">
-      <c r="C308" s="28"/>
+      <c r="C308" s="26"/>
     </row>
     <row r="309" spans="3:3">
-      <c r="C309" s="28"/>
+      <c r="C309" s="26"/>
     </row>
     <row r="310" spans="3:3">
-      <c r="C310" s="28"/>
+      <c r="C310" s="26"/>
     </row>
     <row r="311" spans="3:3">
-      <c r="C311" s="28"/>
+      <c r="C311" s="26"/>
     </row>
     <row r="312" spans="3:3">
-      <c r="C312" s="28"/>
+      <c r="C312" s="26"/>
     </row>
     <row r="313" spans="3:3">
-      <c r="C313" s="28"/>
+      <c r="C313" s="26"/>
     </row>
     <row r="314" spans="3:3">
-      <c r="C314" s="28"/>
+      <c r="C314" s="26"/>
     </row>
     <row r="315" spans="3:3">
-      <c r="C315" s="28"/>
+      <c r="C315" s="26"/>
     </row>
     <row r="316" spans="3:3">
-      <c r="C316" s="28"/>
+      <c r="C316" s="26"/>
     </row>
     <row r="317" spans="3:3">
-      <c r="C317" s="28"/>
+      <c r="C317" s="26"/>
     </row>
     <row r="318" spans="3:3">
-      <c r="C318" s="28"/>
+      <c r="C318" s="26"/>
     </row>
     <row r="319" spans="3:3">
-      <c r="C319" s="28"/>
+      <c r="C319" s="26"/>
     </row>
     <row r="320" spans="3:3">
-      <c r="C320" s="28"/>
+      <c r="C320" s="26"/>
     </row>
     <row r="321" spans="3:3">
-      <c r="C321" s="28"/>
+      <c r="C321" s="26"/>
     </row>
     <row r="322" spans="3:3">
-      <c r="C322" s="28"/>
+      <c r="C322" s="26"/>
     </row>
     <row r="323" spans="3:3">
-      <c r="C323" s="28"/>
+      <c r="C323" s="26"/>
     </row>
     <row r="324" spans="3:3">
-      <c r="C324" s="28"/>
+      <c r="C324" s="26"/>
     </row>
     <row r="325" spans="3:3">
-      <c r="C325" s="28"/>
+      <c r="C325" s="26"/>
     </row>
     <row r="326" spans="3:3">
-      <c r="C326" s="28"/>
+      <c r="C326" s="26"/>
     </row>
     <row r="327" spans="3:3">
-      <c r="C327" s="28"/>
+      <c r="C327" s="26"/>
     </row>
     <row r="328" spans="3:3">
-      <c r="C328" s="28"/>
+      <c r="C328" s="26"/>
     </row>
     <row r="329" spans="3:3">
-      <c r="C329" s="28"/>
+      <c r="C329" s="26"/>
     </row>
     <row r="330" spans="3:3">
-      <c r="C330" s="28"/>
+      <c r="C330" s="26"/>
     </row>
     <row r="331" spans="3:3">
-      <c r="C331" s="28"/>
+      <c r="C331" s="26"/>
     </row>
     <row r="332" spans="3:3">
-      <c r="C332" s="28"/>
+      <c r="C332" s="26"/>
     </row>
     <row r="333" spans="3:3">
-      <c r="C333" s="28"/>
+      <c r="C333" s="26"/>
     </row>
     <row r="334" spans="3:3">
-      <c r="C334" s="28"/>
+      <c r="C334" s="26"/>
     </row>
     <row r="335" spans="3:3">
-      <c r="C335" s="28"/>
+      <c r="C335" s="26"/>
     </row>
     <row r="336" spans="3:3">
-      <c r="C336" s="28"/>
+      <c r="C336" s="26"/>
     </row>
     <row r="337" spans="3:3">
-      <c r="C337" s="28"/>
+      <c r="C337" s="26"/>
     </row>
     <row r="338" spans="3:3">
-      <c r="C338" s="28"/>
+      <c r="C338" s="26"/>
     </row>
     <row r="339" spans="3:3">
-      <c r="C339" s="28"/>
+      <c r="C339" s="26"/>
     </row>
     <row r="340" spans="3:3">
-      <c r="C340" s="28"/>
+      <c r="C340" s="26"/>
     </row>
     <row r="341" spans="3:3">
-      <c r="C341" s="28"/>
+      <c r="C341" s="26"/>
     </row>
     <row r="342" spans="3:3">
-      <c r="C342" s="28"/>
+      <c r="C342" s="26"/>
     </row>
     <row r="343" spans="3:3">
-      <c r="C343" s="28"/>
+      <c r="C343" s="26"/>
     </row>
     <row r="344" spans="3:3">
-      <c r="C344" s="28"/>
+      <c r="C344" s="26"/>
     </row>
     <row r="345" spans="3:3">
-      <c r="C345" s="28"/>
+      <c r="C345" s="26"/>
     </row>
     <row r="346" spans="3:3">
-      <c r="C346" s="28"/>
+      <c r="C346" s="26"/>
     </row>
     <row r="347" spans="3:3">
-      <c r="C347" s="28"/>
+      <c r="C347" s="26"/>
     </row>
     <row r="348" spans="3:3">
-      <c r="C348" s="28"/>
+      <c r="C348" s="26"/>
     </row>
     <row r="349" spans="3:3">
-      <c r="C349" s="28"/>
+      <c r="C349" s="26"/>
     </row>
     <row r="350" spans="3:3">
-      <c r="C350" s="28"/>
+      <c r="C350" s="26"/>
     </row>
     <row r="351" spans="3:3">
-      <c r="C351" s="28"/>
+      <c r="C351" s="26"/>
     </row>
     <row r="352" spans="3:3">
-      <c r="C352" s="28"/>
+      <c r="C352" s="26"/>
     </row>
     <row r="353" spans="3:3">
-      <c r="C353" s="28"/>
+      <c r="C353" s="26"/>
     </row>
     <row r="354" spans="3:3">
-      <c r="C354" s="28"/>
+      <c r="C354" s="26"/>
     </row>
     <row r="355" spans="3:3">
-      <c r="C355" s="28"/>
+      <c r="C355" s="26"/>
     </row>
     <row r="356" spans="3:3">
-      <c r="C356" s="28"/>
+      <c r="C356" s="26"/>
     </row>
     <row r="357" spans="3:3">
-      <c r="C357" s="28"/>
+      <c r="C357" s="26"/>
     </row>
     <row r="358" spans="3:3">
-      <c r="C358" s="28"/>
+      <c r="C358" s="26"/>
     </row>
     <row r="359" spans="3:3">
-      <c r="C359" s="28"/>
+      <c r="C359" s="26"/>
     </row>
     <row r="360" spans="3:3">
-      <c r="C360" s="28"/>
+      <c r="C360" s="26"/>
     </row>
     <row r="361" spans="3:3">
-      <c r="C361" s="28"/>
+      <c r="C361" s="26"/>
     </row>
     <row r="362" spans="3:3">
-      <c r="C362" s="28"/>
+      <c r="C362" s="26"/>
     </row>
     <row r="363" spans="3:3">
-      <c r="C363" s="28"/>
+      <c r="C363" s="26"/>
     </row>
     <row r="364" spans="3:3">
-      <c r="C364" s="28"/>
+      <c r="C364" s="26"/>
     </row>
     <row r="365" spans="3:3">
-      <c r="C365" s="28"/>
+      <c r="C365" s="26"/>
     </row>
     <row r="366" spans="3:3">
-      <c r="C366" s="28"/>
+      <c r="C366" s="26"/>
     </row>
     <row r="367" spans="3:3">
-      <c r="C367" s="28"/>
+      <c r="C367" s="26"/>
     </row>
     <row r="368" spans="3:3">
-      <c r="C368" s="28"/>
+      <c r="C368" s="26"/>
     </row>
     <row r="369" spans="3:3">
-      <c r="C369" s="28"/>
+      <c r="C369" s="26"/>
     </row>
     <row r="370" spans="3:3">
-      <c r="C370" s="28"/>
+      <c r="C370" s="26"/>
     </row>
     <row r="371" spans="3:3">
-      <c r="C371" s="28"/>
+      <c r="C371" s="26"/>
     </row>
     <row r="372" spans="3:3">
-      <c r="C372" s="28"/>
+      <c r="C372" s="26"/>
     </row>
     <row r="373" spans="3:3">
-      <c r="C373" s="28"/>
+      <c r="C373" s="26"/>
     </row>
     <row r="374" spans="3:3">
-      <c r="C374" s="28"/>
+      <c r="C374" s="26"/>
     </row>
     <row r="375" spans="3:3">
-      <c r="C375" s="28"/>
+      <c r="C375" s="26"/>
     </row>
     <row r="376" spans="3:3">
-      <c r="C376" s="28"/>
+      <c r="C376" s="26"/>
     </row>
     <row r="377" spans="3:3">
-      <c r="C377" s="28"/>
+      <c r="C377" s="26"/>
     </row>
     <row r="378" spans="3:3">
-      <c r="C378" s="28"/>
+      <c r="C378" s="26"/>
     </row>
     <row r="379" spans="3:3">
-      <c r="C379" s="28"/>
+      <c r="C379" s="26"/>
     </row>
     <row r="380" spans="3:3">
-      <c r="C380" s="28"/>
+      <c r="C380" s="26"/>
     </row>
     <row r="381" spans="3:3">
-      <c r="C381" s="28"/>
+      <c r="C381" s="26"/>
     </row>
     <row r="382" spans="3:3">
-      <c r="C382" s="28"/>
+      <c r="C382" s="26"/>
     </row>
     <row r="383" spans="3:3">
-      <c r="C383" s="28"/>
+      <c r="C383" s="26"/>
     </row>
     <row r="384" spans="3:3">
-      <c r="C384" s="28"/>
+      <c r="C384" s="26"/>
     </row>
     <row r="385" spans="3:3">
-      <c r="C385" s="28"/>
+      <c r="C385" s="26"/>
     </row>
     <row r="386" spans="3:3">
-      <c r="C386" s="28"/>
+      <c r="C386" s="26"/>
     </row>
     <row r="387" spans="3:3">
-      <c r="C387" s="28"/>
+      <c r="C387" s="26"/>
     </row>
     <row r="388" spans="3:3">
-      <c r="C388" s="28"/>
+      <c r="C388" s="26"/>
     </row>
     <row r="389" spans="3:3">
-      <c r="C389" s="28"/>
+      <c r="C389" s="26"/>
     </row>
     <row r="390" spans="3:3">
-      <c r="C390" s="28"/>
+      <c r="C390" s="26"/>
     </row>
     <row r="391" spans="3:3">
-      <c r="C391" s="28"/>
+      <c r="C391" s="26"/>
     </row>
     <row r="392" spans="3:3">
-      <c r="C392" s="28"/>
+      <c r="C392" s="26"/>
     </row>
     <row r="393" spans="3:3">
-      <c r="C393" s="28"/>
+      <c r="C393" s="26"/>
     </row>
     <row r="394" spans="3:3">
-      <c r="C394" s="28"/>
+      <c r="C394" s="26"/>
     </row>
     <row r="395" spans="3:3">
-      <c r="C395" s="28"/>
+      <c r="C395" s="26"/>
     </row>
     <row r="396" spans="3:3">
-      <c r="C396" s="28"/>
+      <c r="C396" s="26"/>
     </row>
     <row r="397" spans="3:3">
-      <c r="C397" s="28"/>
+      <c r="C397" s="26"/>
     </row>
     <row r="398" spans="3:3">
-      <c r="C398" s="28"/>
+      <c r="C398" s="26"/>
     </row>
     <row r="399" spans="3:3">
-      <c r="C399" s="28"/>
+      <c r="C399" s="26"/>
     </row>
     <row r="400" spans="3:3">
-      <c r="C400" s="28"/>
+      <c r="C400" s="26"/>
     </row>
     <row r="401" spans="3:3">
-      <c r="C401" s="28"/>
+      <c r="C401" s="26"/>
     </row>
     <row r="402" spans="3:3">
-      <c r="C402" s="28"/>
+      <c r="C402" s="26"/>
     </row>
     <row r="403" spans="3:3">
-      <c r="C403" s="28"/>
+      <c r="C403" s="26"/>
     </row>
     <row r="404" spans="3:3">
-      <c r="C404" s="28"/>
+      <c r="C404" s="26"/>
     </row>
     <row r="405" spans="3:3">
-      <c r="C405" s="28"/>
+      <c r="C405" s="26"/>
     </row>
     <row r="406" spans="3:3">
-      <c r="C406" s="28"/>
+      <c r="C406" s="26"/>
     </row>
     <row r="407" spans="3:3">
-      <c r="C407" s="28"/>
+      <c r="C407" s="26"/>
     </row>
     <row r="408" spans="3:3">
-      <c r="C408" s="28"/>
+      <c r="C408" s="26"/>
     </row>
     <row r="409" spans="3:3">
-      <c r="C409" s="28"/>
+      <c r="C409" s="26"/>
     </row>
     <row r="410" spans="3:3">
-      <c r="C410" s="28"/>
+      <c r="C410" s="26"/>
     </row>
     <row r="411" spans="3:3">
-      <c r="C411" s="28"/>
+      <c r="C411" s="26"/>
     </row>
     <row r="412" spans="3:3">
-      <c r="C412" s="28"/>
+      <c r="C412" s="26"/>
     </row>
     <row r="413" spans="3:3">
-      <c r="C413" s="28"/>
+      <c r="C413" s="26"/>
     </row>
     <row r="414" spans="3:3">
-      <c r="C414" s="28"/>
+      <c r="C414" s="26"/>
     </row>
     <row r="415" spans="3:3">
-      <c r="C415" s="28"/>
+      <c r="C415" s="26"/>
     </row>
     <row r="416" spans="3:3">
-      <c r="C416" s="28"/>
+      <c r="C416" s="26"/>
     </row>
     <row r="417" spans="3:3">
-      <c r="C417" s="28"/>
+      <c r="C417" s="26"/>
     </row>
     <row r="418" spans="3:3">
-      <c r="C418" s="28"/>
+      <c r="C418" s="26"/>
     </row>
     <row r="419" spans="3:3">
-      <c r="C419" s="28"/>
+      <c r="C419" s="26"/>
     </row>
     <row r="420" spans="3:3">
-      <c r="C420" s="28"/>
+      <c r="C420" s="26"/>
     </row>
     <row r="421" spans="3:3">
-      <c r="C421" s="28"/>
+      <c r="C421" s="26"/>
     </row>
     <row r="422" spans="3:3">
-      <c r="C422" s="28"/>
+      <c r="C422" s="26"/>
     </row>
     <row r="423" spans="3:3">
-      <c r="C423" s="28"/>
+      <c r="C423" s="26"/>
     </row>
     <row r="424" spans="3:3">
-      <c r="C424" s="28"/>
+      <c r="C424" s="26"/>
     </row>
     <row r="425" spans="3:3">
-      <c r="C425" s="28"/>
+      <c r="C425" s="26"/>
     </row>
     <row r="426" spans="3:3">
-      <c r="C426" s="28"/>
+      <c r="C426" s="26"/>
     </row>
     <row r="434" spans="3:3">
-      <c r="C434" s="33"/>
+      <c r="C434" s="31"/>
     </row>
     <row r="435" spans="3:3">
-      <c r="C435" s="33"/>
+      <c r="C435" s="31"/>
     </row>
     <row r="436" spans="3:3">
-      <c r="C436" s="33"/>
+      <c r="C436" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>